<commit_message>
Change values in table 2 to reflect weekday timetable only
</commit_message>
<xml_diff>
--- a/InputExcel.xlsx
+++ b/InputExcel.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://hatchengineering-my.sharepoint.com/personal/justin_fuentes_hatch_com/Documents/Desktop/Test/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/justinfuentes/Desktop/Coding Projects/Hatch/b21-check/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="21" documentId="13_ncr:1_{FA391B58-98B4-E34A-9BA5-07F28E13B2DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AA7D04F6-DB92-421C-A67C-5CF139EC5A2D}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CBBCBFE-1BE0-594E-858B-6F3A59709AA4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="384" yWindow="384" windowWidth="17484" windowHeight="11712" xr2:uid="{79B376A1-3268-2549-BAEC-B5E1066DF9A0}"/>
+    <workbookView xWindow="380" yWindow="760" windowWidth="17480" windowHeight="14800" xr2:uid="{79B376A1-3268-2549-BAEC-B5E1066DF9A0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="112">
   <si>
     <t>Train_ID</t>
   </si>
@@ -291,9 +291,6 @@
   </si>
   <si>
     <t>VIA75</t>
-  </si>
-  <si>
-    <t>12:13:00</t>
   </si>
   <si>
     <t>VIA73</t>
@@ -730,17 +727,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E298A3A-22C5-B847-8E38-6094955752D9}">
   <dimension ref="A1:G65"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K2" sqref="K2"/>
+    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
+      <selection activeCell="C45" sqref="C45"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="27.3984375" customWidth="1"/>
+    <col min="2" max="2" width="27.33203125" customWidth="1"/>
     <col min="3" max="3" width="23.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -754,16 +751,16 @@
         <v>78</v>
       </c>
       <c r="E1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="F1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="G1" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>76</v>
       </c>
@@ -772,34 +769,34 @@
         <v>77</v>
       </c>
       <c r="E2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="F2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="G2" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>75</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C3" s="2"/>
       <c r="E3" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F3" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="G3" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>39</v>
       </c>
@@ -808,13 +805,13 @@
         <v>54</v>
       </c>
       <c r="E4" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F4" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -823,16 +820,16 @@
       </c>
       <c r="C5" s="1"/>
       <c r="E5" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F5" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="G5" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>42</v>
       </c>
@@ -841,13 +838,13 @@
         <v>56</v>
       </c>
       <c r="E6" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F6" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -856,16 +853,16 @@
       </c>
       <c r="C7" s="1"/>
       <c r="E7" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F7" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="G7" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>44</v>
       </c>
@@ -874,16 +871,16 @@
         <v>58</v>
       </c>
       <c r="E8" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F8" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="G8" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>10</v>
       </c>
@@ -892,13 +889,13 @@
       </c>
       <c r="C9" s="1"/>
       <c r="E9" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F9" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>5</v>
       </c>
@@ -907,16 +904,16 @@
         <v>60</v>
       </c>
       <c r="E10" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F10" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="G10" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>13</v>
       </c>
@@ -928,13 +925,13 @@
         <v>79</v>
       </c>
       <c r="E11" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F11" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>50</v>
       </c>
@@ -946,13 +943,13 @@
         <v>79</v>
       </c>
       <c r="E12" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F12" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>37</v>
       </c>
@@ -964,16 +961,16 @@
         <v>79</v>
       </c>
       <c r="E13" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F13" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="G13" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>8</v>
       </c>
@@ -985,16 +982,16 @@
         <v>79</v>
       </c>
       <c r="E14" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F14" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="G14" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>38</v>
       </c>
@@ -1003,16 +1000,16 @@
         <v>53</v>
       </c>
       <c r="E15" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F15" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="G15" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>11</v>
       </c>
@@ -1021,13 +1018,13 @@
       </c>
       <c r="C16" s="1"/>
       <c r="E16" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F16" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>48</v>
       </c>
@@ -1039,16 +1036,16 @@
         <v>79</v>
       </c>
       <c r="E17" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F17" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="G17" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>16</v>
       </c>
@@ -1057,16 +1054,16 @@
       </c>
       <c r="C18" s="1"/>
       <c r="E18" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F18" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="G18" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>19</v>
       </c>
@@ -1078,16 +1075,16 @@
         <v>79</v>
       </c>
       <c r="E19" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F19" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="G19" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>7</v>
       </c>
@@ -1096,16 +1093,16 @@
       </c>
       <c r="C20" s="1"/>
       <c r="E20" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F20" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="G20" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>9</v>
       </c>
@@ -1114,16 +1111,16 @@
       </c>
       <c r="C21" s="1"/>
       <c r="E21" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F21" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="G21" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>40</v>
       </c>
@@ -1135,13 +1132,13 @@
         <v>79</v>
       </c>
       <c r="E22" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F22" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>43</v>
       </c>
@@ -1150,13 +1147,13 @@
         <v>57</v>
       </c>
       <c r="E23" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F23" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>15</v>
       </c>
@@ -1165,13 +1162,13 @@
       </c>
       <c r="C24" s="1"/>
       <c r="E24" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F24" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>46</v>
       </c>
@@ -1180,16 +1177,16 @@
         <v>61</v>
       </c>
       <c r="E25" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F25" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="G25" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>18</v>
       </c>
@@ -1198,16 +1195,16 @@
       </c>
       <c r="C26" s="1"/>
       <c r="E26" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F26" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="G26" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>12</v>
       </c>
@@ -1219,13 +1216,13 @@
         <v>79</v>
       </c>
       <c r="E27" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F27" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>51</v>
       </c>
@@ -1234,13 +1231,13 @@
         <v>66</v>
       </c>
       <c r="E28" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F28" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>1</v>
       </c>
@@ -1252,13 +1249,13 @@
         <v>79</v>
       </c>
       <c r="E29" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F29" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>45</v>
       </c>
@@ -1267,13 +1264,13 @@
         <v>59</v>
       </c>
       <c r="E30" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F30" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>49</v>
       </c>
@@ -1285,13 +1282,13 @@
         <v>79</v>
       </c>
       <c r="E31" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F31" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>20</v>
       </c>
@@ -1300,16 +1297,16 @@
       </c>
       <c r="C32" s="1"/>
       <c r="E32" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F32" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="G32" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>14</v>
       </c>
@@ -1318,13 +1315,13 @@
       </c>
       <c r="C33" s="1"/>
       <c r="E33" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F33" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>47</v>
       </c>
@@ -1333,16 +1330,16 @@
         <v>62</v>
       </c>
       <c r="E34" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F34" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="G34" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>17</v>
       </c>
@@ -1351,16 +1348,16 @@
       </c>
       <c r="C35" s="1"/>
       <c r="E35" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="F35" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="G35" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>68</v>
       </c>
@@ -1369,13 +1366,13 @@
       </c>
       <c r="C36" s="2"/>
       <c r="E36" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="F36" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>71</v>
       </c>
@@ -1384,16 +1381,16 @@
         <v>73</v>
       </c>
       <c r="E37" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="F37" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="G37" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>74</v>
       </c>
@@ -1402,13 +1399,13 @@
         <v>63</v>
       </c>
       <c r="E38" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="F38" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>70</v>
       </c>
@@ -1417,16 +1414,16 @@
       </c>
       <c r="C39" s="2"/>
       <c r="E39" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="F39" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="G39" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>80</v>
       </c>
@@ -1435,247 +1432,247 @@
         <v>81</v>
       </c>
       <c r="E40" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="F40" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>82</v>
       </c>
       <c r="B41" s="2"/>
       <c r="C41" s="2" t="s">
-        <v>83</v>
+        <v>61</v>
       </c>
       <c r="E41" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="F41" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>84</v>
       </c>
       <c r="B42" s="2"/>
       <c r="C42" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="E42" t="s">
+        <v>107</v>
+      </c>
+      <c r="F42" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
         <v>85</v>
-      </c>
-      <c r="E42" t="s">
-        <v>108</v>
-      </c>
-      <c r="F42" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A43" t="s">
-        <v>86</v>
       </c>
       <c r="B43" s="2"/>
       <c r="C43" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="E43" t="s">
+        <v>107</v>
+      </c>
+      <c r="F43" t="s">
+        <v>109</v>
+      </c>
+      <c r="G43" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
         <v>87</v>
-      </c>
-      <c r="E43" t="s">
-        <v>108</v>
-      </c>
-      <c r="F43" t="s">
-        <v>110</v>
-      </c>
-      <c r="G43" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A44" t="s">
-        <v>88</v>
       </c>
       <c r="B44" s="2"/>
       <c r="C44" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="E44" t="s">
+        <v>107</v>
+      </c>
+      <c r="F44" t="s">
+        <v>109</v>
+      </c>
+      <c r="G44" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
         <v>89</v>
-      </c>
-      <c r="E44" t="s">
-        <v>108</v>
-      </c>
-      <c r="F44" t="s">
-        <v>110</v>
-      </c>
-      <c r="G44" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A45" t="s">
-        <v>90</v>
       </c>
       <c r="B45" s="2"/>
       <c r="C45" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="E45" t="s">
+        <v>107</v>
+      </c>
+      <c r="F45" t="s">
+        <v>109</v>
+      </c>
+      <c r="G45" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
         <v>91</v>
       </c>
-      <c r="E45" t="s">
-        <v>108</v>
-      </c>
-      <c r="F45" t="s">
-        <v>110</v>
-      </c>
-      <c r="G45" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A46" t="s">
+      <c r="B46" s="2" t="s">
         <v>92</v>
-      </c>
-      <c r="B46" s="2" t="s">
-        <v>93</v>
       </c>
       <c r="C46" s="2"/>
       <c r="E46" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="F46" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="G46" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
+        <v>93</v>
+      </c>
+      <c r="B47" s="2" t="s">
         <v>94</v>
-      </c>
-      <c r="B47" s="2" t="s">
-        <v>95</v>
       </c>
       <c r="C47" s="2"/>
       <c r="E47" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="F47" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="G47" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
+        <v>95</v>
+      </c>
+      <c r="B48" s="2" t="s">
         <v>96</v>
-      </c>
-      <c r="B48" s="2" t="s">
-        <v>97</v>
       </c>
       <c r="C48" s="2"/>
       <c r="E48" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="F48" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.3">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
+        <v>97</v>
+      </c>
+      <c r="B49" s="2" t="s">
         <v>98</v>
-      </c>
-      <c r="B49" s="2" t="s">
-        <v>99</v>
       </c>
       <c r="C49" s="2"/>
       <c r="E49" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="F49" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.3">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>41</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C50" s="2"/>
       <c r="E50" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="F50" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.3">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B51" s="2" t="s">
         <v>53</v>
       </c>
       <c r="C51" s="2"/>
       <c r="E51" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="F51" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="G51" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B52" s="2"/>
       <c r="C52" s="2"/>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B53" s="2"/>
       <c r="C53" s="2"/>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B54" s="2"/>
       <c r="C54" s="2"/>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B55" s="2"/>
       <c r="C55" s="2"/>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B56" s="2"/>
       <c r="C56" s="2"/>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B57" s="2"/>
       <c r="C57" s="2"/>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B58" s="2"/>
       <c r="C58" s="2"/>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B59" s="2"/>
       <c r="C59" s="2"/>
     </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B60" s="2"/>
       <c r="C60" s="2"/>
     </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B61" s="2"/>
       <c r="C61" s="2"/>
     </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B62" s="2"/>
       <c r="C62" s="2"/>
     </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B63" s="2"/>
       <c r="C63" s="2"/>
     </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:7" x14ac:dyDescent="0.2">
       <c r="C64" s="2"/>
     </row>
-    <row r="65" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="65" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C65" s="2"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add new select_all collume
</commit_message>
<xml_diff>
--- a/InputExcel.xlsx
+++ b/InputExcel.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10709"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/justinfuentes/Desktop/Coding Projects/Hatch/b21-check/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CBBCBFE-1BE0-594E-858B-6F3A59709AA4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5F77484-89BC-2A44-8611-5CCDC4EF1398}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="760" windowWidth="17480" windowHeight="14800" xr2:uid="{79B376A1-3268-2549-BAEC-B5E1066DF9A0}"/>
+    <workbookView xWindow="3960" yWindow="760" windowWidth="17480" windowHeight="14800" xr2:uid="{79B376A1-3268-2549-BAEC-B5E1066DF9A0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="295" uniqueCount="113">
   <si>
     <t>Train_ID</t>
   </si>
@@ -372,6 +372,9 @@
   </si>
   <si>
     <t>Star Icon</t>
+  </si>
+  <si>
+    <t>select_all</t>
   </si>
 </sst>
 </file>
@@ -725,10 +728,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E298A3A-22C5-B847-8E38-6094955752D9}">
-  <dimension ref="A1:G65"/>
+  <dimension ref="A1:H65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
-      <selection activeCell="C45" sqref="C45"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -737,7 +740,7 @@
     <col min="3" max="3" width="23.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -759,8 +762,11 @@
       <c r="G1" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H1" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>76</v>
       </c>
@@ -777,8 +783,11 @@
       <c r="G2" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H2" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>75</v>
       </c>
@@ -795,8 +804,11 @@
       <c r="G3" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H3" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>39</v>
       </c>
@@ -810,8 +822,11 @@
       <c r="F4" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H4" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -828,8 +843,11 @@
       <c r="G5" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H5" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>42</v>
       </c>
@@ -843,8 +861,11 @@
       <c r="F6" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H6" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -861,8 +882,11 @@
       <c r="G7" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H7" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>44</v>
       </c>
@@ -879,8 +903,11 @@
       <c r="G8" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H8" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>10</v>
       </c>
@@ -894,8 +921,11 @@
       <c r="F9" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H9" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>5</v>
       </c>
@@ -912,8 +942,11 @@
       <c r="G10" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H10" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>13</v>
       </c>
@@ -930,8 +963,11 @@
       <c r="F11" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H11" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>50</v>
       </c>
@@ -948,8 +984,11 @@
       <c r="F12" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H12" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>37</v>
       </c>
@@ -969,8 +1008,11 @@
       <c r="G13" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H13" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>8</v>
       </c>
@@ -990,8 +1032,11 @@
       <c r="G14" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H14" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>38</v>
       </c>
@@ -1008,8 +1053,11 @@
       <c r="G15" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H15" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>11</v>
       </c>
@@ -1023,8 +1071,11 @@
       <c r="F16" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H16" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>48</v>
       </c>
@@ -1044,8 +1095,11 @@
       <c r="G17" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H17" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>16</v>
       </c>
@@ -1062,8 +1116,11 @@
       <c r="G18" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H18" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>19</v>
       </c>
@@ -1083,8 +1140,11 @@
       <c r="G19" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H19" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>7</v>
       </c>
@@ -1101,8 +1161,11 @@
       <c r="G20" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H20" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>9</v>
       </c>
@@ -1119,8 +1182,11 @@
       <c r="G21" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H21" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>40</v>
       </c>
@@ -1137,8 +1203,11 @@
       <c r="F22" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H22" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>43</v>
       </c>
@@ -1152,8 +1221,11 @@
       <c r="F23" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H23" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>15</v>
       </c>
@@ -1167,8 +1239,11 @@
       <c r="F24" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H24" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>46</v>
       </c>
@@ -1185,8 +1260,11 @@
       <c r="G25" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H25" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>18</v>
       </c>
@@ -1203,8 +1281,11 @@
       <c r="G26" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H26" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>12</v>
       </c>
@@ -1221,8 +1302,11 @@
       <c r="F27" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H27" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>51</v>
       </c>
@@ -1236,8 +1320,11 @@
       <c r="F28" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H28" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>1</v>
       </c>
@@ -1254,8 +1341,11 @@
       <c r="F29" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H29" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>45</v>
       </c>
@@ -1269,8 +1359,11 @@
       <c r="F30" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H30" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>49</v>
       </c>
@@ -1287,8 +1380,11 @@
       <c r="F31" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H31" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>20</v>
       </c>
@@ -1305,8 +1401,11 @@
       <c r="G32" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H32" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>14</v>
       </c>
@@ -1320,8 +1419,11 @@
       <c r="F33" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H33" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>47</v>
       </c>
@@ -1338,8 +1440,11 @@
       <c r="G34" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H34" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>17</v>
       </c>
@@ -1356,8 +1461,11 @@
       <c r="G35" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H35" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>68</v>
       </c>
@@ -1371,8 +1479,11 @@
       <c r="F36" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H36" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>71</v>
       </c>
@@ -1389,8 +1500,11 @@
       <c r="G37" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H37" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>74</v>
       </c>
@@ -1404,8 +1518,11 @@
       <c r="F38" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H38" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>70</v>
       </c>
@@ -1422,8 +1539,11 @@
       <c r="G39" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H39" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>80</v>
       </c>
@@ -1437,8 +1557,11 @@
       <c r="F40" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H40" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>82</v>
       </c>
@@ -1452,8 +1575,11 @@
       <c r="F41" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H41" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>84</v>
       </c>
@@ -1467,8 +1593,11 @@
       <c r="F42" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H42" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>85</v>
       </c>
@@ -1485,8 +1614,11 @@
       <c r="G43" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H43" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>87</v>
       </c>
@@ -1503,8 +1635,11 @@
       <c r="G44" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H44" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>89</v>
       </c>
@@ -1521,8 +1656,11 @@
       <c r="G45" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H45" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>91</v>
       </c>
@@ -1539,8 +1677,11 @@
       <c r="G46" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H46" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>93</v>
       </c>
@@ -1557,8 +1698,11 @@
       <c r="G47" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H47" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>95</v>
       </c>
@@ -1572,8 +1716,11 @@
       <c r="F48" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H48" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>97</v>
       </c>
@@ -1587,8 +1734,11 @@
       <c r="F49" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H49" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>41</v>
       </c>
@@ -1602,8 +1752,11 @@
       <c r="F50" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H50" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>100</v>
       </c>
@@ -1620,56 +1773,59 @@
       <c r="G51" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H51" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B52" s="2"/>
       <c r="C52" s="2"/>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B53" s="2"/>
       <c r="C53" s="2"/>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B54" s="2"/>
       <c r="C54" s="2"/>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B55" s="2"/>
       <c r="C55" s="2"/>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B56" s="2"/>
       <c r="C56" s="2"/>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B57" s="2"/>
       <c r="C57" s="2"/>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B58" s="2"/>
       <c r="C58" s="2"/>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B59" s="2"/>
       <c r="C59" s="2"/>
     </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B60" s="2"/>
       <c r="C60" s="2"/>
     </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B61" s="2"/>
       <c r="C61" s="2"/>
     </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B62" s="2"/>
       <c r="C62" s="2"/>
     </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B63" s="2"/>
       <c r="C63" s="2"/>
     </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C64" s="2"/>
     </row>
     <row r="65" spans="3:3" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Add day indicator to trains
</commit_message>
<xml_diff>
--- a/InputExcel.xlsx
+++ b/InputExcel.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/justinfuentes/Desktop/Coding Projects/Hatch/b21-check/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5F77484-89BC-2A44-8611-5CCDC4EF1398}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68390E06-2FAB-954C-842D-F472E5C06AEE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3960" yWindow="760" windowWidth="17480" windowHeight="14800" xr2:uid="{79B376A1-3268-2549-BAEC-B5E1066DF9A0}"/>
+    <workbookView xWindow="3960" yWindow="760" windowWidth="21520" windowHeight="17560" xr2:uid="{79B376A1-3268-2549-BAEC-B5E1066DF9A0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="295" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="346" uniqueCount="117">
   <si>
     <t>Train_ID</t>
   </si>
@@ -137,9 +137,6 @@
     <t>19:09:00</t>
   </si>
   <si>
-    <t>21:15:00</t>
-  </si>
-  <si>
     <t>21:45:00</t>
   </si>
   <si>
@@ -375,6 +372,21 @@
   </si>
   <si>
     <t>select_all</t>
+  </si>
+  <si>
+    <t>Train_Type</t>
+  </si>
+  <si>
+    <t>Special</t>
+  </si>
+  <si>
+    <t>BusinessDay</t>
+  </si>
+  <si>
+    <t>21:34:00</t>
+  </si>
+  <si>
+    <t>Ignore</t>
   </si>
 </sst>
 </file>
@@ -728,10 +740,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E298A3A-22C5-B847-8E38-6094955752D9}">
-  <dimension ref="A1:H65"/>
+  <dimension ref="A1:I65"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
+    <sheetView tabSelected="1" zoomScale="114" workbookViewId="0">
+      <selection activeCell="A45" sqref="A45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -740,7 +752,7 @@
     <col min="3" max="3" width="23.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -751,82 +763,94 @@
         <v>3</v>
       </c>
       <c r="D1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="G1" t="s">
+        <v>110</v>
+      </c>
+      <c r="H1" t="s">
         <v>111</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B2" s="2"/>
       <c r="C2" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E2" t="s">
+        <v>101</v>
+      </c>
+      <c r="F2" t="s">
+        <v>108</v>
+      </c>
+      <c r="G2" t="s">
+        <v>78</v>
+      </c>
+      <c r="H2" t="s">
+        <v>78</v>
+      </c>
+      <c r="I2" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>74</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>102</v>
-      </c>
-      <c r="F2" t="s">
-        <v>109</v>
-      </c>
-      <c r="G2" t="s">
-        <v>79</v>
-      </c>
-      <c r="H2" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>75</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>103</v>
       </c>
       <c r="C3" s="2"/>
       <c r="E3" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="F3" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="G3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="H3" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+        <v>78</v>
+      </c>
+      <c r="I3" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B4" s="2"/>
       <c r="C4" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E4" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="F4" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="H4" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+        <v>78</v>
+      </c>
+      <c r="I4" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -835,37 +859,43 @@
       </c>
       <c r="C5" s="1"/>
       <c r="E5" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="F5" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="G5" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="H5" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+        <v>78</v>
+      </c>
+      <c r="I5" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B6" s="2"/>
       <c r="C6" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E6" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="F6" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="H6" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+        <v>78</v>
+      </c>
+      <c r="I6" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -874,40 +904,46 @@
       </c>
       <c r="C7" s="1"/>
       <c r="E7" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="F7" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="G7" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="H7" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+        <v>78</v>
+      </c>
+      <c r="I7" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B8" s="2"/>
       <c r="C8" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E8" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="F8" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="G8" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="H8" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+        <v>78</v>
+      </c>
+      <c r="I8" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>10</v>
       </c>
@@ -916,37 +952,43 @@
       </c>
       <c r="C9" s="1"/>
       <c r="E9" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="F9" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="H9" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+        <v>78</v>
+      </c>
+      <c r="I9" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>5</v>
       </c>
       <c r="B10" s="2"/>
       <c r="C10" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E10" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="F10" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="G10" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="H10" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+        <v>78</v>
+      </c>
+      <c r="I10" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>13</v>
       </c>
@@ -955,64 +997,73 @@
       </c>
       <c r="C11" s="1"/>
       <c r="D11" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E11" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="F11" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="H11" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+        <v>78</v>
+      </c>
+      <c r="I11" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B12" s="2"/>
       <c r="C12" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D12" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E12" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="F12" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="H12" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+        <v>78</v>
+      </c>
+      <c r="I12" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B13" s="2"/>
       <c r="C13" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D13" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E13" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="F13" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="G13" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="H13" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+        <v>78</v>
+      </c>
+      <c r="I13" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>8</v>
       </c>
@@ -1021,43 +1072,49 @@
       </c>
       <c r="C14" s="1"/>
       <c r="D14" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E14" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="F14" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="G14" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="H14" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+        <v>78</v>
+      </c>
+      <c r="I14" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B15" s="2"/>
       <c r="C15" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E15" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="F15" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="G15" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="H15" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+        <v>78</v>
+      </c>
+      <c r="I15" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>11</v>
       </c>
@@ -1066,85 +1123,97 @@
       </c>
       <c r="C16" s="1"/>
       <c r="E16" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="F16" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="H16" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+        <v>78</v>
+      </c>
+      <c r="I16" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B17" s="2"/>
       <c r="C17" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D17" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E17" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="F17" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="G17" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="H17" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+        <v>78</v>
+      </c>
+      <c r="I17" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>16</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C18" s="1"/>
       <c r="E18" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="F18" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="G18" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="H18" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+        <v>78</v>
+      </c>
+      <c r="I18" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>19</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C19" s="1"/>
       <c r="D19" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E19" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="F19" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="G19" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="H19" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+        <v>78</v>
+      </c>
+      <c r="I19" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>7</v>
       </c>
@@ -1153,19 +1222,22 @@
       </c>
       <c r="C20" s="1"/>
       <c r="E20" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="F20" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="G20" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="H20" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+        <v>78</v>
+      </c>
+      <c r="I20" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>9</v>
       </c>
@@ -1174,58 +1246,67 @@
       </c>
       <c r="C21" s="1"/>
       <c r="E21" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="F21" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="G21" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="H21" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+        <v>78</v>
+      </c>
+      <c r="I21" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B22" s="2"/>
       <c r="C22" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D22" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E22" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="F22" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="H22" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+        <v>78</v>
+      </c>
+      <c r="I22" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B23" s="2"/>
       <c r="C23" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E23" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="F23" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="H23" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
+        <v>78</v>
+      </c>
+      <c r="I23" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>15</v>
       </c>
@@ -1234,58 +1315,67 @@
       </c>
       <c r="C24" s="1"/>
       <c r="E24" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="F24" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="H24" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
+        <v>78</v>
+      </c>
+      <c r="I24" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B25" s="2"/>
       <c r="C25" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E25" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="F25" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="G25" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="H25" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
+        <v>78</v>
+      </c>
+      <c r="I25" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>18</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C26" s="1"/>
       <c r="E26" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="F26" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="G26" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="H26" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
+        <v>78</v>
+      </c>
+      <c r="I26" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>12</v>
       </c>
@@ -1294,37 +1384,43 @@
       </c>
       <c r="C27" s="1"/>
       <c r="D27" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E27" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="F27" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="H27" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
+        <v>78</v>
+      </c>
+      <c r="I27" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B28" s="2"/>
       <c r="C28" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E28" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="F28" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="H28" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
+        <v>78</v>
+      </c>
+      <c r="I28" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>1</v>
       </c>
@@ -1333,79 +1429,91 @@
       </c>
       <c r="C29" s="1"/>
       <c r="D29" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E29" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="F29" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="H29" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
+        <v>78</v>
+      </c>
+      <c r="I29" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B30" s="2"/>
       <c r="C30" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E30" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="F30" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="H30" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
+        <v>78</v>
+      </c>
+      <c r="I30" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B31" s="2"/>
       <c r="C31" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D31" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E31" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="F31" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="H31" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
+        <v>78</v>
+      </c>
+      <c r="I31" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>20</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C32" s="1"/>
       <c r="E32" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="F32" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="G32" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="H32" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
+        <v>78</v>
+      </c>
+      <c r="I32" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>14</v>
       </c>
@@ -1414,418 +1522,475 @@
       </c>
       <c r="C33" s="1"/>
       <c r="E33" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="F33" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="H33" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
+        <v>78</v>
+      </c>
+      <c r="I33" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B34" s="2"/>
       <c r="C34" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E34" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="F34" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="G34" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="H34" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
+        <v>78</v>
+      </c>
+      <c r="I34" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>17</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>33</v>
+        <v>115</v>
       </c>
       <c r="C35" s="1"/>
       <c r="E35" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F35" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="G35" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="H35" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
+        <v>78</v>
+      </c>
+      <c r="I35" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
+        <v>67</v>
+      </c>
+      <c r="B36" s="2" t="s">
         <v>68</v>
-      </c>
-      <c r="B36" s="2" t="s">
-        <v>69</v>
       </c>
       <c r="C36" s="2"/>
       <c r="E36" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F36" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="H36" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
+        <v>78</v>
+      </c>
+      <c r="I36" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B37" s="2"/>
       <c r="C37" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="E37" t="s">
+        <v>104</v>
+      </c>
+      <c r="F37" t="s">
+        <v>108</v>
+      </c>
+      <c r="G37" t="s">
+        <v>78</v>
+      </c>
+      <c r="H37" t="s">
+        <v>78</v>
+      </c>
+      <c r="I37" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
         <v>73</v>
-      </c>
-      <c r="E37" t="s">
-        <v>105</v>
-      </c>
-      <c r="F37" t="s">
-        <v>109</v>
-      </c>
-      <c r="G37" t="s">
-        <v>79</v>
-      </c>
-      <c r="H37" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A38" t="s">
-        <v>74</v>
       </c>
       <c r="B38" s="2"/>
       <c r="C38" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E38" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F38" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="H38" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
+        <v>78</v>
+      </c>
+      <c r="I38" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C39" s="2"/>
       <c r="E39" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F39" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="G39" t="s">
+        <v>78</v>
+      </c>
+      <c r="H39" t="s">
+        <v>78</v>
+      </c>
+      <c r="I39" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
         <v>79</v>
-      </c>
-      <c r="H39" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A40" t="s">
-        <v>80</v>
       </c>
       <c r="B40" s="2"/>
       <c r="C40" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="E40" t="s">
+        <v>106</v>
+      </c>
+      <c r="F40" t="s">
+        <v>108</v>
+      </c>
+      <c r="H40" t="s">
+        <v>78</v>
+      </c>
+      <c r="I40" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
         <v>81</v>
-      </c>
-      <c r="E40" t="s">
-        <v>107</v>
-      </c>
-      <c r="F40" t="s">
-        <v>109</v>
-      </c>
-      <c r="H40" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A41" t="s">
-        <v>82</v>
       </c>
       <c r="B41" s="2"/>
       <c r="C41" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E41" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F41" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="H41" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.2">
+        <v>78</v>
+      </c>
+      <c r="I41" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B42" s="2"/>
       <c r="C42" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E42" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F42" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="H42" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.2">
+        <v>78</v>
+      </c>
+      <c r="I42" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B43" s="2"/>
       <c r="C43" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="E43" t="s">
+        <v>106</v>
+      </c>
+      <c r="F43" t="s">
+        <v>108</v>
+      </c>
+      <c r="G43" t="s">
+        <v>78</v>
+      </c>
+      <c r="H43" t="s">
+        <v>78</v>
+      </c>
+      <c r="I43" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
         <v>86</v>
-      </c>
-      <c r="E43" t="s">
-        <v>107</v>
-      </c>
-      <c r="F43" t="s">
-        <v>109</v>
-      </c>
-      <c r="G43" t="s">
-        <v>79</v>
-      </c>
-      <c r="H43" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A44" t="s">
-        <v>87</v>
       </c>
       <c r="B44" s="2"/>
       <c r="C44" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="E44" t="s">
+        <v>106</v>
+      </c>
+      <c r="F44" t="s">
+        <v>108</v>
+      </c>
+      <c r="G44" t="s">
+        <v>78</v>
+      </c>
+      <c r="H44" t="s">
+        <v>78</v>
+      </c>
+      <c r="I44" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
         <v>88</v>
-      </c>
-      <c r="E44" t="s">
-        <v>107</v>
-      </c>
-      <c r="F44" t="s">
-        <v>109</v>
-      </c>
-      <c r="G44" t="s">
-        <v>79</v>
-      </c>
-      <c r="H44" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A45" t="s">
-        <v>89</v>
       </c>
       <c r="B45" s="2"/>
       <c r="C45" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="E45" t="s">
+        <v>106</v>
+      </c>
+      <c r="F45" t="s">
+        <v>108</v>
+      </c>
+      <c r="G45" t="s">
+        <v>78</v>
+      </c>
+      <c r="H45" t="s">
+        <v>78</v>
+      </c>
+      <c r="I45" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
         <v>90</v>
       </c>
-      <c r="E45" t="s">
-        <v>107</v>
-      </c>
-      <c r="F45" t="s">
-        <v>109</v>
-      </c>
-      <c r="G45" t="s">
-        <v>79</v>
-      </c>
-      <c r="H45" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A46" t="s">
+      <c r="B46" s="2" t="s">
         <v>91</v>
-      </c>
-      <c r="B46" s="2" t="s">
-        <v>92</v>
       </c>
       <c r="C46" s="2"/>
       <c r="E46" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F46" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="G46" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="H46" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.2">
+        <v>78</v>
+      </c>
+      <c r="I46" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
+        <v>92</v>
+      </c>
+      <c r="B47" s="2" t="s">
         <v>93</v>
-      </c>
-      <c r="B47" s="2" t="s">
-        <v>94</v>
       </c>
       <c r="C47" s="2"/>
       <c r="E47" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F47" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="G47" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="H47" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.2">
+        <v>78</v>
+      </c>
+      <c r="I47" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
+        <v>94</v>
+      </c>
+      <c r="B48" s="2" t="s">
         <v>95</v>
-      </c>
-      <c r="B48" s="2" t="s">
-        <v>96</v>
       </c>
       <c r="C48" s="2"/>
       <c r="E48" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F48" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="H48" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.2">
+        <v>78</v>
+      </c>
+      <c r="I48" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
+        <v>96</v>
+      </c>
+      <c r="B49" s="2" t="s">
         <v>97</v>
-      </c>
-      <c r="B49" s="2" t="s">
-        <v>98</v>
       </c>
       <c r="C49" s="2"/>
       <c r="E49" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F49" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="H49" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.2">
+        <v>78</v>
+      </c>
+      <c r="I49" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C50" s="2"/>
       <c r="E50" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F50" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="H50" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.2">
+        <v>78</v>
+      </c>
+      <c r="I50" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C51" s="2"/>
       <c r="E51" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F51" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="G51" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="H51" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.2">
+        <v>78</v>
+      </c>
+      <c r="I51" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B52" s="2"/>
       <c r="C52" s="2"/>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B53" s="2"/>
       <c r="C53" s="2"/>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B54" s="2"/>
       <c r="C54" s="2"/>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B55" s="2"/>
       <c r="C55" s="2"/>
     </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B56" s="2"/>
       <c r="C56" s="2"/>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B57" s="2"/>
       <c r="C57" s="2"/>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B58" s="2"/>
       <c r="C58" s="2"/>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B59" s="2"/>
       <c r="C59" s="2"/>
     </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B60" s="2"/>
       <c r="C60" s="2"/>
     </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B61" s="2"/>
       <c r="C61" s="2"/>
     </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B62" s="2"/>
       <c r="C62" s="2"/>
     </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B63" s="2"/>
       <c r="C63" s="2"/>
     </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:9" x14ac:dyDescent="0.2">
       <c r="C64" s="2"/>
     </row>
     <row r="65" spans="3:3" x14ac:dyDescent="0.2">
@@ -1835,7 +2000,7 @@
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C39">
     <sortCondition ref="A1:A39"/>
   </sortState>
-  <dataValidations count="4">
+  <dataValidations count="5">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E1" xr:uid="{21FFFA42-49BF-654D-973B-24FD3A7A6AC9}">
       <formula1>"Table 1,Table 2,Table 3,Table 4,Table 5, Table 6,Table 7"</formula1>
     </dataValidation>
@@ -1848,6 +2013,9 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G1048576" xr:uid="{D8696CB5-2EF9-EE46-9890-299C7E2A49B1}">
       <formula1>"yes"</formula1>
     </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I2:I102" xr:uid="{91EAA47F-B2BD-0E4B-803E-80401D46D9FC}">
+      <formula1>"Special,Both,BusinessDay,Ignore"</formula1>
+    </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>

<commit_message>
change / to %
</commit_message>
<xml_diff>
--- a/InputExcel.xlsx
+++ b/InputExcel.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/justinfuentes/Desktop/Coding Projects/Hatch/b21-check/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68390E06-2FAB-954C-842D-F472E5C06AEE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D96A8F8-CED6-C34B-AFF5-7B34033E4A60}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3960" yWindow="760" windowWidth="21520" windowHeight="17560" xr2:uid="{79B376A1-3268-2549-BAEC-B5E1066DF9A0}"/>
   </bookViews>
@@ -146,12 +146,6 @@
     <t>23:33:00</t>
   </si>
   <si>
-    <t>VIA50/60</t>
-  </si>
-  <si>
-    <t>VIA52/62</t>
-  </si>
-  <si>
     <t>VIA40</t>
   </si>
   <si>
@@ -387,6 +381,12 @@
   </si>
   <si>
     <t>Ignore</t>
+  </si>
+  <si>
+    <t>VIA50&amp;60</t>
+  </si>
+  <si>
+    <t>VIA52&amp;62</t>
   </si>
 </sst>
 </file>
@@ -742,8 +742,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E298A3A-22C5-B847-8E38-6094955752D9}">
   <dimension ref="A1:I65"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="114" workbookViewId="0">
-      <selection activeCell="A45" sqref="A45"/>
+    <sheetView tabSelected="1" topLeftCell="A36" zoomScale="114" workbookViewId="0">
+      <selection activeCell="G55" sqref="G55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -763,91 +763,91 @@
         <v>3</v>
       </c>
       <c r="D1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="E1" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="F1" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="G1" t="s">
+        <v>108</v>
+      </c>
+      <c r="H1" t="s">
+        <v>109</v>
+      </c>
+      <c r="I1" t="s">
         <v>110</v>
-      </c>
-      <c r="H1" t="s">
-        <v>111</v>
-      </c>
-      <c r="I1" t="s">
-        <v>112</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B2" s="2"/>
       <c r="C2" s="2" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="E2" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="F2" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="G2" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="H2" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="I2" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C3" s="2"/>
       <c r="E3" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="F3" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="G3" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="H3" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="I3" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B4" s="2"/>
       <c r="C4" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="E4" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="F4" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="H4" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="I4" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
@@ -859,40 +859,40 @@
       </c>
       <c r="C5" s="1"/>
       <c r="E5" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="F5" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="G5" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="H5" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="I5" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B6" s="2"/>
       <c r="C6" s="2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E6" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="F6" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="H6" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="I6" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
@@ -904,43 +904,43 @@
       </c>
       <c r="C7" s="1"/>
       <c r="E7" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="F7" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="G7" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="H7" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="I7" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B8" s="2"/>
       <c r="C8" s="2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="E8" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="F8" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="G8" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="H8" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="I8" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
@@ -952,16 +952,16 @@
       </c>
       <c r="C9" s="1"/>
       <c r="E9" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="F9" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="H9" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="I9" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
@@ -970,22 +970,22 @@
       </c>
       <c r="B10" s="2"/>
       <c r="C10" s="2" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="E10" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="F10" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="G10" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="H10" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="I10" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
@@ -997,70 +997,70 @@
       </c>
       <c r="C11" s="1"/>
       <c r="D11" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="E11" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="F11" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="H11" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="I11" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B12" s="2"/>
       <c r="C12" s="2" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D12" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="E12" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="F12" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="H12" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="I12" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>36</v>
+        <v>115</v>
       </c>
       <c r="B13" s="2"/>
       <c r="C13" s="2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D13" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="E13" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="F13" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="G13" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="H13" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="I13" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.2">
@@ -1072,46 +1072,46 @@
       </c>
       <c r="C14" s="1"/>
       <c r="D14" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="E14" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="F14" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="G14" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="H14" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="I14" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>37</v>
+        <v>116</v>
       </c>
       <c r="B15" s="2"/>
       <c r="C15" s="2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="E15" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="F15" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="G15" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="H15" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="I15" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.2">
@@ -1123,43 +1123,43 @@
       </c>
       <c r="C16" s="1"/>
       <c r="E16" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="F16" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="H16" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="I16" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B17" s="2"/>
       <c r="C17" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D17" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="E17" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="F17" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="G17" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="H17" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="I17" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.2">
@@ -1167,23 +1167,23 @@
         <v>16</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C18" s="1"/>
       <c r="E18" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="F18" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="G18" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="H18" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="I18" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.2">
@@ -1195,22 +1195,22 @@
       </c>
       <c r="C19" s="1"/>
       <c r="D19" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="E19" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="F19" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="G19" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="H19" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="I19" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.2">
@@ -1222,19 +1222,19 @@
       </c>
       <c r="C20" s="1"/>
       <c r="E20" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="F20" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="G20" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="H20" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="I20" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.2">
@@ -1246,64 +1246,64 @@
       </c>
       <c r="C21" s="1"/>
       <c r="E21" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="F21" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="G21" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="H21" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="I21" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B22" s="2"/>
       <c r="C22" s="2" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D22" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="E22" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="F22" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="H22" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="I22" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B23" s="2"/>
       <c r="C23" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="E23" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="F23" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="H23" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="I23" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.2">
@@ -1315,40 +1315,40 @@
       </c>
       <c r="C24" s="1"/>
       <c r="E24" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="F24" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="H24" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="I24" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B25" s="2"/>
       <c r="C25" s="2" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E25" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="F25" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="G25" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="H25" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="I25" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.2">
@@ -1360,19 +1360,19 @@
       </c>
       <c r="C26" s="1"/>
       <c r="E26" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="F26" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="G26" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="H26" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="I26" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.2">
@@ -1384,40 +1384,40 @@
       </c>
       <c r="C27" s="1"/>
       <c r="D27" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="E27" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="F27" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="H27" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="I27" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B28" s="2"/>
       <c r="C28" s="2" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="E28" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="F28" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="H28" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="I28" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.2">
@@ -1429,64 +1429,64 @@
       </c>
       <c r="C29" s="1"/>
       <c r="D29" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="E29" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="F29" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="H29" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="I29" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B30" s="2"/>
       <c r="C30" s="2" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="E30" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="F30" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="H30" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="I30" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B31" s="2"/>
       <c r="C31" s="2" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D31" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="E31" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="F31" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="H31" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="I31" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.2">
@@ -1498,19 +1498,19 @@
       </c>
       <c r="C32" s="1"/>
       <c r="E32" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="F32" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="G32" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="H32" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="I32" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.2">
@@ -1522,40 +1522,40 @@
       </c>
       <c r="C33" s="1"/>
       <c r="E33" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="F33" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="H33" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="I33" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B34" s="2"/>
       <c r="C34" s="2" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="E34" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="F34" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="G34" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="H34" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="I34" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.2">
@@ -1563,383 +1563,383 @@
         <v>17</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="C35" s="1"/>
       <c r="E35" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="F35" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="G35" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="H35" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="I35" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C36" s="2"/>
       <c r="E36" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="F36" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="H36" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="I36" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B37" s="2"/>
       <c r="C37" s="2" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="E37" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="F37" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="G37" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="H37" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="I37" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B38" s="2"/>
       <c r="C38" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="E38" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="F38" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="H38" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="I38" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
+        <v>67</v>
+      </c>
+      <c r="B39" s="2" t="s">
         <v>69</v>
-      </c>
-      <c r="B39" s="2" t="s">
-        <v>71</v>
       </c>
       <c r="C39" s="2"/>
       <c r="E39" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="F39" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="G39" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="H39" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="I39" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B40" s="2"/>
       <c r="C40" s="2" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="E40" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="F40" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="H40" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="I40" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B41" s="2"/>
       <c r="C41" s="2" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E41" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="F41" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="H41" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="I41" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B42" s="2"/>
       <c r="C42" s="2" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="E42" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="F42" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="H42" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="I42" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B43" s="2"/>
       <c r="C43" s="2" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="E43" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="F43" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="G43" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="H43" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="I43" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B44" s="2"/>
       <c r="C44" s="2" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="E44" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="F44" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="G44" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="H44" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="I44" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B45" s="2"/>
       <c r="C45" s="2" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="E45" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="F45" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="G45" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="H45" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="I45" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C46" s="2"/>
       <c r="E46" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="F46" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="G46" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="H46" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="I46" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C47" s="2"/>
       <c r="E47" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="F47" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="G47" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="H47" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="I47" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C48" s="2"/>
       <c r="E48" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="F48" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="H48" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="I48" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C49" s="2"/>
       <c r="E49" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="F49" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="H49" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="I49" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C50" s="2"/>
       <c r="E50" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="F50" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="H50" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="I50" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C51" s="2"/>
       <c r="E51" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="F51" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="G51" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="H51" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="I51" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Changed Both to just weekday
</commit_message>
<xml_diff>
--- a/InputExcel.xlsx
+++ b/InputExcel.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/justinfuentes/Desktop/Coding Projects/Hatch/b21-check/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D96A8F8-CED6-C34B-AFF5-7B34033E4A60}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94E0556C-05EE-0741-88B6-1555342C5FE0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3960" yWindow="760" windowWidth="21520" windowHeight="17560" xr2:uid="{79B376A1-3268-2549-BAEC-B5E1066DF9A0}"/>
+    <workbookView xWindow="4580" yWindow="1520" windowWidth="21520" windowHeight="17560" xr2:uid="{79B376A1-3268-2549-BAEC-B5E1066DF9A0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="346" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="346" uniqueCount="116">
   <si>
     <t>Train_ID</t>
   </si>
@@ -369,9 +370,6 @@
   </si>
   <si>
     <t>Train_Type</t>
-  </si>
-  <si>
-    <t>Special</t>
   </si>
   <si>
     <t>BusinessDay</t>
@@ -402,12 +400,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -422,10 +426,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -742,8 +747,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E298A3A-22C5-B847-8E38-6094955752D9}">
   <dimension ref="A1:I65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A36" zoomScale="114" workbookViewId="0">
-      <selection activeCell="G55" sqref="G55"/>
+    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="J36" sqref="J36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -802,7 +807,7 @@
         <v>76</v>
       </c>
       <c r="I2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
@@ -826,7 +831,7 @@
         <v>76</v>
       </c>
       <c r="I3" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
@@ -847,7 +852,7 @@
         <v>76</v>
       </c>
       <c r="I4" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
@@ -871,7 +876,7 @@
         <v>76</v>
       </c>
       <c r="I5" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
@@ -892,7 +897,7 @@
         <v>76</v>
       </c>
       <c r="I6" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
@@ -916,7 +921,7 @@
         <v>76</v>
       </c>
       <c r="I7" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
@@ -940,7 +945,7 @@
         <v>76</v>
       </c>
       <c r="I8" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
@@ -961,7 +966,7 @@
         <v>76</v>
       </c>
       <c r="I9" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
@@ -985,7 +990,7 @@
         <v>76</v>
       </c>
       <c r="I10" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
@@ -1009,7 +1014,7 @@
         <v>76</v>
       </c>
       <c r="I11" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
@@ -1033,12 +1038,12 @@
         <v>76</v>
       </c>
       <c r="I12" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B13" s="2"/>
       <c r="C13" s="2" t="s">
@@ -1060,7 +1065,7 @@
         <v>76</v>
       </c>
       <c r="I13" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.2">
@@ -1087,12 +1092,12 @@
         <v>76</v>
       </c>
       <c r="I14" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B15" s="2"/>
       <c r="C15" s="2" t="s">
@@ -1111,7 +1116,7 @@
         <v>76</v>
       </c>
       <c r="I15" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.2">
@@ -1132,7 +1137,7 @@
         <v>76</v>
       </c>
       <c r="I16" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.2">
@@ -1159,7 +1164,7 @@
         <v>76</v>
       </c>
       <c r="I17" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.2">
@@ -1183,7 +1188,7 @@
         <v>76</v>
       </c>
       <c r="I18" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.2">
@@ -1210,7 +1215,7 @@
         <v>76</v>
       </c>
       <c r="I19" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.2">
@@ -1234,7 +1239,7 @@
         <v>76</v>
       </c>
       <c r="I20" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.2">
@@ -1258,7 +1263,7 @@
         <v>76</v>
       </c>
       <c r="I21" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.2">
@@ -1282,7 +1287,7 @@
         <v>76</v>
       </c>
       <c r="I22" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.2">
@@ -1303,7 +1308,7 @@
         <v>76</v>
       </c>
       <c r="I23" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.2">
@@ -1324,7 +1329,7 @@
         <v>76</v>
       </c>
       <c r="I24" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.2">
@@ -1348,7 +1353,7 @@
         <v>76</v>
       </c>
       <c r="I25" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.2">
@@ -1372,7 +1377,7 @@
         <v>76</v>
       </c>
       <c r="I26" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.2">
@@ -1396,7 +1401,7 @@
         <v>76</v>
       </c>
       <c r="I27" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.2">
@@ -1417,7 +1422,7 @@
         <v>76</v>
       </c>
       <c r="I28" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.2">
@@ -1441,7 +1446,7 @@
         <v>76</v>
       </c>
       <c r="I29" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.2">
@@ -1462,7 +1467,7 @@
         <v>76</v>
       </c>
       <c r="I30" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.2">
@@ -1486,7 +1491,7 @@
         <v>76</v>
       </c>
       <c r="I31" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.2">
@@ -1510,7 +1515,7 @@
         <v>76</v>
       </c>
       <c r="I32" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.2">
@@ -1531,7 +1536,7 @@
         <v>76</v>
       </c>
       <c r="I33" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.2">
@@ -1555,7 +1560,7 @@
         <v>76</v>
       </c>
       <c r="I34" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.2">
@@ -1563,7 +1568,7 @@
         <v>17</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C35" s="1"/>
       <c r="E35" t="s">
@@ -1579,11 +1584,11 @@
         <v>76</v>
       </c>
       <c r="I35" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A36" t="s">
+      <c r="A36" s="3" t="s">
         <v>65</v>
       </c>
       <c r="B36" s="2" t="s">
@@ -1604,7 +1609,7 @@
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A37" t="s">
+      <c r="A37" s="3" t="s">
         <v>68</v>
       </c>
       <c r="B37" s="2"/>
@@ -1628,7 +1633,7 @@
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A38" t="s">
+      <c r="A38" s="3" t="s">
         <v>71</v>
       </c>
       <c r="B38" s="2"/>
@@ -1649,7 +1654,7 @@
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A39" t="s">
+      <c r="A39" s="3" t="s">
         <v>67</v>
       </c>
       <c r="B39" s="2" t="s">
@@ -1690,7 +1695,7 @@
         <v>76</v>
       </c>
       <c r="I40" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.2">
@@ -1711,7 +1716,7 @@
         <v>76</v>
       </c>
       <c r="I41" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.2">
@@ -1732,7 +1737,7 @@
         <v>76</v>
       </c>
       <c r="I42" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.2">
@@ -1756,7 +1761,7 @@
         <v>76</v>
       </c>
       <c r="I43" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.2">
@@ -1780,7 +1785,7 @@
         <v>76</v>
       </c>
       <c r="I44" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.2">
@@ -1804,7 +1809,7 @@
         <v>76</v>
       </c>
       <c r="I45" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.2">
@@ -1828,7 +1833,7 @@
         <v>76</v>
       </c>
       <c r="I46" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.2">
@@ -1852,7 +1857,7 @@
         <v>76</v>
       </c>
       <c r="I47" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.2">
@@ -1873,7 +1878,7 @@
         <v>76</v>
       </c>
       <c r="I48" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.2">
@@ -1894,7 +1899,7 @@
         <v>76</v>
       </c>
       <c r="I49" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.2">
@@ -1915,7 +1920,7 @@
         <v>76</v>
       </c>
       <c r="I50" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.2">
@@ -1939,7 +1944,7 @@
         <v>76</v>
       </c>
       <c r="I51" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.2">
@@ -2020,4 +2025,16 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CBC6D709-B491-AA47-BA6A-A4E51D62D65F}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Update from new reqs from excel
</commit_message>
<xml_diff>
--- a/InputExcel.xlsx
+++ b/InputExcel.xlsx
@@ -8,14 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/justinfuentes/Desktop/Coding Projects/Hatch/b21-check/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94E0556C-05EE-0741-88B6-1555342C5FE0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26643C36-35D3-114D-B240-1FBA2B442266}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4580" yWindow="1520" windowWidth="21520" windowHeight="17560" xr2:uid="{79B376A1-3268-2549-BAEC-B5E1066DF9A0}"/>
+    <workbookView xWindow="4580" yWindow="1260" windowWidth="21520" windowHeight="17560" xr2:uid="{79B376A1-3268-2549-BAEC-B5E1066DF9A0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$I$51</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -37,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="346" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="352" uniqueCount="119">
   <si>
     <t>Train_ID</t>
   </si>
@@ -108,9 +111,6 @@
     <t>10:02:00</t>
   </si>
   <si>
-    <t>11:24:00</t>
-  </si>
-  <si>
     <t>11:46:00</t>
   </si>
   <si>
@@ -129,15 +129,6 @@
     <t>17:15:00</t>
   </si>
   <si>
-    <t>18:30:00</t>
-  </si>
-  <si>
-    <t>16:17:00</t>
-  </si>
-  <si>
-    <t>19:09:00</t>
-  </si>
-  <si>
     <t>21:45:00</t>
   </si>
   <si>
@@ -192,45 +183,12 @@
     <t>08:35:00</t>
   </si>
   <si>
-    <t>10:40:00</t>
-  </si>
-  <si>
-    <t>11:30:00</t>
-  </si>
-  <si>
-    <t>12:20:00</t>
-  </si>
-  <si>
-    <t>13:20:00</t>
-  </si>
-  <si>
-    <t>14:20:00</t>
-  </si>
-  <si>
-    <t>15:15:00</t>
-  </si>
-  <si>
-    <t>15:40:00</t>
-  </si>
-  <si>
     <t>16:35:00</t>
   </si>
   <si>
-    <t>17:00:00</t>
-  </si>
-  <si>
     <t>17:40:00</t>
   </si>
   <si>
-    <t>18:07:00</t>
-  </si>
-  <si>
-    <t>18:40:00</t>
-  </si>
-  <si>
-    <t>19:35:00</t>
-  </si>
-  <si>
     <t>19:57:00</t>
   </si>
   <si>
@@ -306,21 +264,12 @@
     <t>VIA78</t>
   </si>
   <si>
-    <t>21:51:00</t>
-  </si>
-  <si>
     <t>VIA98</t>
   </si>
   <si>
-    <t>19:41:00</t>
-  </si>
-  <si>
     <t>VIA76</t>
   </si>
   <si>
-    <t>17:52:00</t>
-  </si>
-  <si>
     <t>VIA70</t>
   </si>
   <si>
@@ -375,9 +324,6 @@
     <t>BusinessDay</t>
   </si>
   <si>
-    <t>21:34:00</t>
-  </si>
-  <si>
     <t>Ignore</t>
   </si>
   <si>
@@ -385,6 +331,72 @@
   </si>
   <si>
     <t>VIA52&amp;62</t>
+  </si>
+  <si>
+    <t>11:25:00</t>
+  </si>
+  <si>
+    <t>16:18:00</t>
+  </si>
+  <si>
+    <t>18:33:00</t>
+  </si>
+  <si>
+    <t>19:03:00</t>
+  </si>
+  <si>
+    <t>21:15:00</t>
+  </si>
+  <si>
+    <t>08:32:00</t>
+  </si>
+  <si>
+    <t>10:32:00</t>
+  </si>
+  <si>
+    <t>11:32:00</t>
+  </si>
+  <si>
+    <t>12:17:00</t>
+  </si>
+  <si>
+    <t>13:17:00</t>
+  </si>
+  <si>
+    <t>14:17:00</t>
+  </si>
+  <si>
+    <t>15:17:00</t>
+  </si>
+  <si>
+    <t>15:32:00</t>
+  </si>
+  <si>
+    <t>16:32:00</t>
+  </si>
+  <si>
+    <t>17:02:00</t>
+  </si>
+  <si>
+    <t>17:32:00</t>
+  </si>
+  <si>
+    <t>18:02:00</t>
+  </si>
+  <si>
+    <t>18:32:00</t>
+  </si>
+  <si>
+    <t>19:32:00</t>
+  </si>
+  <si>
+    <t>17:53:00</t>
+  </si>
+  <si>
+    <t>19:43:00</t>
+  </si>
+  <si>
+    <t>21:50:00</t>
   </si>
 </sst>
 </file>
@@ -747,8 +759,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E298A3A-22C5-B847-8E38-6094955752D9}">
   <dimension ref="A1:I65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="J36" sqref="J36"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -768,91 +780,94 @@
         <v>3</v>
       </c>
       <c r="D1" t="s">
-        <v>75</v>
+        <v>60</v>
       </c>
       <c r="E1" t="s">
-        <v>98</v>
+        <v>80</v>
       </c>
       <c r="F1" t="s">
-        <v>105</v>
+        <v>87</v>
       </c>
       <c r="G1" t="s">
-        <v>108</v>
+        <v>90</v>
       </c>
       <c r="H1" t="s">
-        <v>109</v>
+        <v>91</v>
       </c>
       <c r="I1" t="s">
-        <v>110</v>
+        <v>92</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>73</v>
+        <v>58</v>
       </c>
       <c r="B2" s="2"/>
       <c r="C2" s="2" t="s">
-        <v>74</v>
+        <v>59</v>
       </c>
       <c r="E2" t="s">
-        <v>99</v>
+        <v>81</v>
       </c>
       <c r="F2" t="s">
-        <v>106</v>
+        <v>88</v>
       </c>
       <c r="G2" t="s">
-        <v>76</v>
+        <v>61</v>
       </c>
       <c r="H2" t="s">
-        <v>76</v>
+        <v>61</v>
       </c>
       <c r="I2" t="s">
-        <v>113</v>
+        <v>94</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>72</v>
+        <v>57</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>100</v>
+        <v>82</v>
       </c>
       <c r="C3" s="2"/>
       <c r="E3" t="s">
-        <v>101</v>
+        <v>83</v>
       </c>
       <c r="F3" t="s">
-        <v>107</v>
+        <v>89</v>
       </c>
       <c r="G3" t="s">
-        <v>76</v>
+        <v>61</v>
       </c>
       <c r="H3" t="s">
-        <v>76</v>
+        <v>61</v>
       </c>
       <c r="I3" t="s">
-        <v>113</v>
+        <v>94</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="B4" s="2"/>
       <c r="C4" s="2" t="s">
-        <v>51</v>
+        <v>103</v>
+      </c>
+      <c r="D4" t="s">
+        <v>61</v>
       </c>
       <c r="E4" t="s">
-        <v>103</v>
+        <v>85</v>
       </c>
       <c r="F4" t="s">
-        <v>106</v>
+        <v>88</v>
       </c>
       <c r="H4" t="s">
-        <v>76</v>
+        <v>61</v>
       </c>
       <c r="I4" t="s">
-        <v>111</v>
+        <v>93</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
@@ -864,40 +879,40 @@
       </c>
       <c r="C5" s="1"/>
       <c r="E5" t="s">
-        <v>103</v>
+        <v>85</v>
       </c>
       <c r="F5" t="s">
-        <v>107</v>
-      </c>
-      <c r="G5" t="s">
-        <v>76</v>
+        <v>89</v>
       </c>
       <c r="H5" t="s">
-        <v>76</v>
+        <v>61</v>
       </c>
       <c r="I5" t="s">
-        <v>111</v>
+        <v>93</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="B6" s="2"/>
       <c r="C6" s="2" t="s">
-        <v>53</v>
+        <v>105</v>
+      </c>
+      <c r="D6" t="s">
+        <v>61</v>
       </c>
       <c r="E6" t="s">
-        <v>103</v>
+        <v>85</v>
       </c>
       <c r="F6" t="s">
-        <v>106</v>
+        <v>88</v>
       </c>
       <c r="H6" t="s">
-        <v>76</v>
+        <v>61</v>
       </c>
       <c r="I6" t="s">
-        <v>111</v>
+        <v>93</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
@@ -905,47 +920,53 @@
         <v>6</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>23</v>
+        <v>97</v>
       </c>
       <c r="C7" s="1"/>
+      <c r="D7" t="s">
+        <v>61</v>
+      </c>
       <c r="E7" t="s">
-        <v>103</v>
+        <v>85</v>
       </c>
       <c r="F7" t="s">
-        <v>107</v>
+        <v>89</v>
       </c>
       <c r="G7" t="s">
-        <v>76</v>
+        <v>61</v>
       </c>
       <c r="H7" t="s">
-        <v>76</v>
+        <v>61</v>
       </c>
       <c r="I7" t="s">
-        <v>111</v>
+        <v>93</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="B8" s="2"/>
       <c r="C8" s="2" t="s">
-        <v>55</v>
+        <v>107</v>
+      </c>
+      <c r="D8" t="s">
+        <v>61</v>
       </c>
       <c r="E8" t="s">
-        <v>103</v>
+        <v>85</v>
       </c>
       <c r="F8" t="s">
-        <v>106</v>
+        <v>88</v>
       </c>
       <c r="G8" t="s">
-        <v>76</v>
+        <v>61</v>
       </c>
       <c r="H8" t="s">
-        <v>76</v>
+        <v>61</v>
       </c>
       <c r="I8" t="s">
-        <v>111</v>
+        <v>93</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
@@ -953,20 +974,20 @@
         <v>10</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C9" s="1"/>
       <c r="E9" t="s">
-        <v>103</v>
+        <v>85</v>
       </c>
       <c r="F9" t="s">
-        <v>107</v>
+        <v>89</v>
       </c>
       <c r="H9" t="s">
-        <v>76</v>
+        <v>61</v>
       </c>
       <c r="I9" t="s">
-        <v>111</v>
+        <v>93</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
@@ -975,22 +996,25 @@
       </c>
       <c r="B10" s="2"/>
       <c r="C10" s="2" t="s">
-        <v>57</v>
+        <v>109</v>
+      </c>
+      <c r="D10" t="s">
+        <v>61</v>
       </c>
       <c r="E10" t="s">
-        <v>103</v>
+        <v>85</v>
       </c>
       <c r="F10" t="s">
-        <v>106</v>
+        <v>88</v>
       </c>
       <c r="G10" t="s">
-        <v>76</v>
+        <v>61</v>
       </c>
       <c r="H10" t="s">
-        <v>76</v>
+        <v>61</v>
       </c>
       <c r="I10" t="s">
-        <v>111</v>
+        <v>93</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
@@ -998,74 +1022,71 @@
         <v>13</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C11" s="1"/>
-      <c r="D11" t="s">
-        <v>76</v>
-      </c>
       <c r="E11" t="s">
-        <v>103</v>
+        <v>85</v>
       </c>
       <c r="F11" t="s">
-        <v>107</v>
+        <v>89</v>
       </c>
       <c r="H11" t="s">
-        <v>76</v>
+        <v>61</v>
       </c>
       <c r="I11" t="s">
-        <v>111</v>
+        <v>93</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="B12" s="2"/>
       <c r="C12" s="2" t="s">
-        <v>62</v>
+        <v>114</v>
       </c>
       <c r="D12" t="s">
-        <v>76</v>
+        <v>61</v>
       </c>
       <c r="E12" t="s">
-        <v>103</v>
+        <v>85</v>
       </c>
       <c r="F12" t="s">
-        <v>106</v>
+        <v>88</v>
       </c>
       <c r="H12" t="s">
-        <v>76</v>
+        <v>61</v>
       </c>
       <c r="I12" t="s">
-        <v>111</v>
+        <v>93</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>114</v>
+        <v>95</v>
       </c>
       <c r="B13" s="2"/>
       <c r="C13" s="2" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="D13" t="s">
-        <v>76</v>
+        <v>61</v>
       </c>
       <c r="E13" t="s">
-        <v>103</v>
+        <v>85</v>
       </c>
       <c r="F13" t="s">
-        <v>106</v>
+        <v>88</v>
       </c>
       <c r="G13" t="s">
-        <v>76</v>
+        <v>61</v>
       </c>
       <c r="H13" t="s">
-        <v>76</v>
+        <v>61</v>
       </c>
       <c r="I13" t="s">
-        <v>111</v>
+        <v>93</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.2">
@@ -1073,50 +1094,47 @@
         <v>8</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C14" s="1"/>
-      <c r="D14" t="s">
-        <v>76</v>
-      </c>
       <c r="E14" t="s">
-        <v>103</v>
+        <v>85</v>
       </c>
       <c r="F14" t="s">
-        <v>107</v>
+        <v>89</v>
       </c>
       <c r="G14" t="s">
-        <v>76</v>
+        <v>61</v>
       </c>
       <c r="H14" t="s">
-        <v>76</v>
+        <v>61</v>
       </c>
       <c r="I14" t="s">
-        <v>111</v>
+        <v>93</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>115</v>
+        <v>96</v>
       </c>
       <c r="B15" s="2"/>
       <c r="C15" s="2" t="s">
-        <v>50</v>
+        <v>102</v>
+      </c>
+      <c r="D15" t="s">
+        <v>61</v>
       </c>
       <c r="E15" t="s">
-        <v>103</v>
+        <v>85</v>
       </c>
       <c r="F15" t="s">
-        <v>106</v>
-      </c>
-      <c r="G15" t="s">
-        <v>76</v>
+        <v>88</v>
       </c>
       <c r="H15" t="s">
-        <v>76</v>
+        <v>61</v>
       </c>
       <c r="I15" t="s">
-        <v>111</v>
+        <v>93</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.2">
@@ -1124,47 +1142,47 @@
         <v>11</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C16" s="1"/>
       <c r="E16" t="s">
-        <v>103</v>
+        <v>85</v>
       </c>
       <c r="F16" t="s">
-        <v>107</v>
+        <v>89</v>
       </c>
       <c r="H16" t="s">
-        <v>76</v>
+        <v>61</v>
       </c>
       <c r="I16" t="s">
-        <v>111</v>
+        <v>93</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="B17" s="2"/>
       <c r="C17" s="2" t="s">
-        <v>60</v>
+        <v>112</v>
       </c>
       <c r="D17" t="s">
-        <v>76</v>
+        <v>61</v>
       </c>
       <c r="E17" t="s">
-        <v>103</v>
+        <v>85</v>
       </c>
       <c r="F17" t="s">
-        <v>106</v>
+        <v>88</v>
       </c>
       <c r="G17" t="s">
-        <v>76</v>
+        <v>61</v>
       </c>
       <c r="H17" t="s">
-        <v>76</v>
+        <v>61</v>
       </c>
       <c r="I17" t="s">
-        <v>111</v>
+        <v>93</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.2">
@@ -1172,23 +1190,23 @@
         <v>16</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>64</v>
+        <v>49</v>
       </c>
       <c r="C18" s="1"/>
       <c r="E18" t="s">
-        <v>103</v>
+        <v>85</v>
       </c>
       <c r="F18" t="s">
-        <v>107</v>
+        <v>89</v>
       </c>
       <c r="G18" t="s">
-        <v>76</v>
+        <v>61</v>
       </c>
       <c r="H18" t="s">
-        <v>76</v>
+        <v>61</v>
       </c>
       <c r="I18" t="s">
-        <v>111</v>
+        <v>93</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.2">
@@ -1196,26 +1214,26 @@
         <v>19</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="C19" s="1"/>
       <c r="D19" t="s">
-        <v>76</v>
+        <v>61</v>
       </c>
       <c r="E19" t="s">
-        <v>103</v>
+        <v>85</v>
       </c>
       <c r="F19" t="s">
-        <v>107</v>
+        <v>89</v>
       </c>
       <c r="G19" t="s">
-        <v>76</v>
+        <v>61</v>
       </c>
       <c r="H19" t="s">
-        <v>76</v>
+        <v>61</v>
       </c>
       <c r="I19" t="s">
-        <v>111</v>
+        <v>93</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.2">
@@ -1223,23 +1241,23 @@
         <v>7</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C20" s="1"/>
       <c r="E20" t="s">
-        <v>103</v>
+        <v>85</v>
       </c>
       <c r="F20" t="s">
-        <v>107</v>
+        <v>89</v>
       </c>
       <c r="G20" t="s">
-        <v>76</v>
+        <v>61</v>
       </c>
       <c r="H20" t="s">
-        <v>76</v>
+        <v>61</v>
       </c>
       <c r="I20" t="s">
-        <v>111</v>
+        <v>93</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.2">
@@ -1247,68 +1265,71 @@
         <v>9</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C21" s="1"/>
       <c r="E21" t="s">
-        <v>103</v>
+        <v>85</v>
       </c>
       <c r="F21" t="s">
-        <v>107</v>
+        <v>89</v>
       </c>
       <c r="G21" t="s">
-        <v>76</v>
+        <v>61</v>
       </c>
       <c r="H21" t="s">
-        <v>76</v>
+        <v>61</v>
       </c>
       <c r="I21" t="s">
-        <v>111</v>
+        <v>93</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="B22" s="2"/>
       <c r="C22" s="2" t="s">
-        <v>52</v>
+        <v>104</v>
       </c>
       <c r="D22" t="s">
-        <v>76</v>
+        <v>61</v>
       </c>
       <c r="E22" t="s">
-        <v>103</v>
+        <v>85</v>
       </c>
       <c r="F22" t="s">
-        <v>106</v>
+        <v>88</v>
       </c>
       <c r="H22" t="s">
-        <v>76</v>
+        <v>61</v>
       </c>
       <c r="I22" t="s">
-        <v>111</v>
+        <v>93</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="B23" s="2"/>
       <c r="C23" s="2" t="s">
-        <v>54</v>
+        <v>106</v>
+      </c>
+      <c r="D23" t="s">
+        <v>61</v>
       </c>
       <c r="E23" t="s">
-        <v>103</v>
+        <v>85</v>
       </c>
       <c r="F23" t="s">
-        <v>106</v>
+        <v>88</v>
       </c>
       <c r="H23" t="s">
-        <v>76</v>
+        <v>61</v>
       </c>
       <c r="I23" t="s">
-        <v>111</v>
+        <v>93</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.2">
@@ -1316,44 +1337,44 @@
         <v>15</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>32</v>
+        <v>100</v>
       </c>
       <c r="C24" s="1"/>
       <c r="E24" t="s">
-        <v>103</v>
+        <v>85</v>
       </c>
       <c r="F24" t="s">
-        <v>107</v>
+        <v>89</v>
       </c>
       <c r="H24" t="s">
-        <v>76</v>
+        <v>61</v>
       </c>
       <c r="I24" t="s">
-        <v>111</v>
+        <v>93</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="B25" s="2"/>
       <c r="C25" s="2" t="s">
-        <v>58</v>
+        <v>110</v>
       </c>
       <c r="E25" t="s">
-        <v>103</v>
+        <v>85</v>
       </c>
       <c r="F25" t="s">
-        <v>106</v>
+        <v>88</v>
       </c>
       <c r="G25" t="s">
-        <v>76</v>
+        <v>61</v>
       </c>
       <c r="H25" t="s">
-        <v>76</v>
+        <v>61</v>
       </c>
       <c r="I25" t="s">
-        <v>111</v>
+        <v>93</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.2">
@@ -1361,23 +1382,26 @@
         <v>18</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="C26" s="1"/>
+      <c r="D26" t="s">
+        <v>61</v>
+      </c>
       <c r="E26" t="s">
-        <v>103</v>
+        <v>85</v>
       </c>
       <c r="F26" t="s">
-        <v>107</v>
+        <v>89</v>
       </c>
       <c r="G26" t="s">
-        <v>76</v>
+        <v>61</v>
       </c>
       <c r="H26" t="s">
-        <v>76</v>
+        <v>61</v>
       </c>
       <c r="I26" t="s">
-        <v>111</v>
+        <v>93</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.2">
@@ -1385,44 +1409,44 @@
         <v>12</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>31</v>
+        <v>98</v>
       </c>
       <c r="C27" s="1"/>
       <c r="D27" t="s">
-        <v>76</v>
+        <v>61</v>
       </c>
       <c r="E27" t="s">
-        <v>103</v>
+        <v>85</v>
       </c>
       <c r="F27" t="s">
-        <v>107</v>
+        <v>89</v>
       </c>
       <c r="H27" t="s">
-        <v>76</v>
+        <v>61</v>
       </c>
       <c r="I27" t="s">
-        <v>111</v>
+        <v>93</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="B28" s="2"/>
       <c r="C28" s="2" t="s">
-        <v>63</v>
+        <v>115</v>
       </c>
       <c r="E28" t="s">
-        <v>103</v>
+        <v>85</v>
       </c>
       <c r="F28" t="s">
-        <v>106</v>
+        <v>88</v>
       </c>
       <c r="H28" t="s">
-        <v>76</v>
+        <v>61</v>
       </c>
       <c r="I28" t="s">
-        <v>111</v>
+        <v>93</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.2">
@@ -1434,64 +1458,67 @@
       </c>
       <c r="C29" s="1"/>
       <c r="D29" t="s">
-        <v>76</v>
+        <v>61</v>
       </c>
       <c r="E29" t="s">
-        <v>103</v>
+        <v>85</v>
       </c>
       <c r="F29" t="s">
-        <v>107</v>
+        <v>89</v>
       </c>
       <c r="H29" t="s">
-        <v>76</v>
+        <v>61</v>
       </c>
       <c r="I29" t="s">
-        <v>111</v>
+        <v>93</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="B30" s="2"/>
       <c r="C30" s="2" t="s">
-        <v>56</v>
+        <v>108</v>
+      </c>
+      <c r="D30" t="s">
+        <v>61</v>
       </c>
       <c r="E30" t="s">
-        <v>103</v>
+        <v>85</v>
       </c>
       <c r="F30" t="s">
-        <v>106</v>
+        <v>88</v>
       </c>
       <c r="H30" t="s">
-        <v>76</v>
+        <v>61</v>
       </c>
       <c r="I30" t="s">
-        <v>111</v>
+        <v>93</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="B31" s="2"/>
       <c r="C31" s="2" t="s">
-        <v>61</v>
+        <v>113</v>
       </c>
       <c r="D31" t="s">
-        <v>76</v>
+        <v>61</v>
       </c>
       <c r="E31" t="s">
-        <v>103</v>
+        <v>85</v>
       </c>
       <c r="F31" t="s">
-        <v>106</v>
+        <v>88</v>
       </c>
       <c r="H31" t="s">
-        <v>76</v>
+        <v>61</v>
       </c>
       <c r="I31" t="s">
-        <v>111</v>
+        <v>93</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.2">
@@ -1499,23 +1526,23 @@
         <v>20</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="C32" s="1"/>
       <c r="E32" t="s">
-        <v>103</v>
+        <v>85</v>
       </c>
       <c r="F32" t="s">
-        <v>107</v>
+        <v>89</v>
       </c>
       <c r="G32" t="s">
-        <v>76</v>
+        <v>61</v>
       </c>
       <c r="H32" t="s">
-        <v>76</v>
+        <v>61</v>
       </c>
       <c r="I32" t="s">
-        <v>111</v>
+        <v>93</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.2">
@@ -1523,44 +1550,47 @@
         <v>14</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>30</v>
+        <v>99</v>
       </c>
       <c r="C33" s="1"/>
       <c r="E33" t="s">
-        <v>103</v>
+        <v>85</v>
       </c>
       <c r="F33" t="s">
-        <v>107</v>
+        <v>89</v>
       </c>
       <c r="H33" t="s">
-        <v>76</v>
+        <v>61</v>
       </c>
       <c r="I33" t="s">
-        <v>111</v>
+        <v>93</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="B34" s="2"/>
       <c r="C34" s="2" t="s">
-        <v>59</v>
+        <v>111</v>
+      </c>
+      <c r="D34" t="s">
+        <v>61</v>
       </c>
       <c r="E34" t="s">
-        <v>103</v>
+        <v>85</v>
       </c>
       <c r="F34" t="s">
-        <v>106</v>
+        <v>88</v>
       </c>
       <c r="G34" t="s">
-        <v>76</v>
+        <v>61</v>
       </c>
       <c r="H34" t="s">
-        <v>76</v>
+        <v>61</v>
       </c>
       <c r="I34" t="s">
-        <v>111</v>
+        <v>93</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.2">
@@ -1568,383 +1598,383 @@
         <v>17</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>112</v>
+        <v>101</v>
       </c>
       <c r="C35" s="1"/>
       <c r="E35" t="s">
-        <v>104</v>
+        <v>85</v>
       </c>
       <c r="F35" t="s">
-        <v>106</v>
+        <v>89</v>
       </c>
       <c r="G35" t="s">
-        <v>76</v>
+        <v>61</v>
       </c>
       <c r="H35" t="s">
-        <v>76</v>
+        <v>61</v>
       </c>
       <c r="I35" t="s">
-        <v>111</v>
+        <v>93</v>
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A36" s="3" t="s">
-        <v>65</v>
+        <v>50</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>66</v>
+        <v>51</v>
       </c>
       <c r="C36" s="2"/>
       <c r="E36" t="s">
-        <v>102</v>
+        <v>84</v>
       </c>
       <c r="F36" t="s">
-        <v>107</v>
+        <v>89</v>
       </c>
       <c r="H36" t="s">
-        <v>76</v>
+        <v>61</v>
       </c>
       <c r="I36" t="s">
-        <v>111</v>
+        <v>93</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A37" s="3" t="s">
-        <v>68</v>
+        <v>53</v>
       </c>
       <c r="B37" s="2"/>
       <c r="C37" s="2" t="s">
-        <v>70</v>
+        <v>55</v>
       </c>
       <c r="E37" t="s">
-        <v>102</v>
+        <v>84</v>
       </c>
       <c r="F37" t="s">
-        <v>106</v>
+        <v>88</v>
       </c>
       <c r="G37" t="s">
-        <v>76</v>
+        <v>61</v>
       </c>
       <c r="H37" t="s">
-        <v>76</v>
+        <v>61</v>
       </c>
       <c r="I37" t="s">
-        <v>111</v>
+        <v>93</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A38" s="3" t="s">
-        <v>71</v>
+        <v>56</v>
       </c>
       <c r="B38" s="2"/>
       <c r="C38" s="2" t="s">
-        <v>60</v>
+        <v>48</v>
       </c>
       <c r="E38" t="s">
-        <v>102</v>
+        <v>84</v>
       </c>
       <c r="F38" t="s">
-        <v>106</v>
+        <v>88</v>
       </c>
       <c r="H38" t="s">
-        <v>76</v>
+        <v>61</v>
       </c>
       <c r="I38" t="s">
-        <v>111</v>
+        <v>93</v>
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A39" s="3" t="s">
-        <v>67</v>
+        <v>52</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>69</v>
+        <v>54</v>
       </c>
       <c r="C39" s="2"/>
       <c r="E39" t="s">
-        <v>102</v>
+        <v>84</v>
       </c>
       <c r="F39" t="s">
-        <v>107</v>
+        <v>89</v>
       </c>
       <c r="G39" t="s">
-        <v>76</v>
+        <v>61</v>
       </c>
       <c r="H39" t="s">
-        <v>76</v>
+        <v>61</v>
       </c>
       <c r="I39" t="s">
-        <v>111</v>
+        <v>93</v>
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>77</v>
+        <v>62</v>
       </c>
       <c r="B40" s="2"/>
       <c r="C40" s="2" t="s">
-        <v>78</v>
+        <v>63</v>
       </c>
       <c r="E40" t="s">
-        <v>104</v>
+        <v>86</v>
       </c>
       <c r="F40" t="s">
-        <v>106</v>
+        <v>88</v>
       </c>
       <c r="H40" t="s">
-        <v>76</v>
+        <v>61</v>
       </c>
       <c r="I40" t="s">
-        <v>111</v>
+        <v>93</v>
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>79</v>
+        <v>64</v>
       </c>
       <c r="B41" s="2"/>
       <c r="C41" s="2" t="s">
-        <v>58</v>
+        <v>47</v>
       </c>
       <c r="E41" t="s">
-        <v>104</v>
+        <v>86</v>
       </c>
       <c r="F41" t="s">
-        <v>106</v>
+        <v>88</v>
       </c>
       <c r="H41" t="s">
-        <v>76</v>
+        <v>61</v>
       </c>
       <c r="I41" t="s">
-        <v>111</v>
+        <v>93</v>
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>81</v>
+        <v>66</v>
       </c>
       <c r="B42" s="2"/>
       <c r="C42" s="2" t="s">
-        <v>80</v>
+        <v>65</v>
       </c>
       <c r="E42" t="s">
-        <v>104</v>
+        <v>86</v>
       </c>
       <c r="F42" t="s">
-        <v>106</v>
+        <v>88</v>
       </c>
       <c r="H42" t="s">
-        <v>76</v>
+        <v>61</v>
       </c>
       <c r="I42" t="s">
-        <v>111</v>
+        <v>93</v>
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>82</v>
+        <v>67</v>
       </c>
       <c r="B43" s="2"/>
       <c r="C43" s="2" t="s">
-        <v>83</v>
+        <v>68</v>
       </c>
       <c r="E43" t="s">
-        <v>104</v>
+        <v>86</v>
       </c>
       <c r="F43" t="s">
-        <v>106</v>
+        <v>88</v>
       </c>
       <c r="G43" t="s">
-        <v>76</v>
+        <v>61</v>
       </c>
       <c r="H43" t="s">
-        <v>76</v>
+        <v>61</v>
       </c>
       <c r="I43" t="s">
-        <v>111</v>
+        <v>93</v>
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>84</v>
+        <v>69</v>
       </c>
       <c r="B44" s="2"/>
       <c r="C44" s="2" t="s">
-        <v>85</v>
+        <v>70</v>
       </c>
       <c r="E44" t="s">
-        <v>104</v>
+        <v>86</v>
       </c>
       <c r="F44" t="s">
-        <v>106</v>
+        <v>88</v>
       </c>
       <c r="G44" t="s">
-        <v>76</v>
+        <v>61</v>
       </c>
       <c r="H44" t="s">
-        <v>76</v>
+        <v>61</v>
       </c>
       <c r="I44" t="s">
-        <v>111</v>
+        <v>93</v>
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>86</v>
+        <v>71</v>
       </c>
       <c r="B45" s="2"/>
       <c r="C45" s="2" t="s">
-        <v>87</v>
+        <v>72</v>
       </c>
       <c r="E45" t="s">
-        <v>104</v>
+        <v>86</v>
       </c>
       <c r="F45" t="s">
-        <v>106</v>
+        <v>88</v>
       </c>
       <c r="G45" t="s">
-        <v>76</v>
+        <v>61</v>
       </c>
       <c r="H45" t="s">
-        <v>76</v>
+        <v>61</v>
       </c>
       <c r="I45" t="s">
-        <v>111</v>
+        <v>93</v>
       </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>88</v>
+        <v>73</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>89</v>
+        <v>118</v>
       </c>
       <c r="C46" s="2"/>
       <c r="E46" t="s">
-        <v>104</v>
+        <v>86</v>
       </c>
       <c r="F46" t="s">
-        <v>107</v>
+        <v>89</v>
       </c>
       <c r="G46" t="s">
-        <v>76</v>
+        <v>61</v>
       </c>
       <c r="H46" t="s">
-        <v>76</v>
+        <v>61</v>
       </c>
       <c r="I46" t="s">
-        <v>111</v>
+        <v>93</v>
       </c>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>90</v>
+        <v>74</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>91</v>
+        <v>117</v>
       </c>
       <c r="C47" s="2"/>
       <c r="E47" t="s">
-        <v>104</v>
+        <v>86</v>
       </c>
       <c r="F47" t="s">
-        <v>107</v>
+        <v>89</v>
       </c>
       <c r="G47" t="s">
-        <v>76</v>
+        <v>61</v>
       </c>
       <c r="H47" t="s">
-        <v>76</v>
+        <v>61</v>
       </c>
       <c r="I47" t="s">
-        <v>111</v>
+        <v>93</v>
       </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>92</v>
+        <v>75</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>93</v>
+        <v>116</v>
       </c>
       <c r="C48" s="2"/>
       <c r="E48" t="s">
-        <v>104</v>
+        <v>86</v>
       </c>
       <c r="F48" t="s">
-        <v>107</v>
+        <v>89</v>
       </c>
       <c r="H48" t="s">
-        <v>76</v>
+        <v>61</v>
       </c>
       <c r="I48" t="s">
-        <v>111</v>
+        <v>93</v>
       </c>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>94</v>
+        <v>76</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>95</v>
+        <v>77</v>
       </c>
       <c r="C49" s="2"/>
       <c r="E49" t="s">
-        <v>104</v>
+        <v>86</v>
       </c>
       <c r="F49" t="s">
-        <v>107</v>
+        <v>89</v>
       </c>
       <c r="H49" t="s">
-        <v>76</v>
+        <v>61</v>
       </c>
       <c r="I49" t="s">
-        <v>111</v>
+        <v>93</v>
       </c>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>96</v>
+        <v>78</v>
       </c>
       <c r="C50" s="2"/>
       <c r="E50" t="s">
-        <v>104</v>
+        <v>86</v>
       </c>
       <c r="F50" t="s">
-        <v>107</v>
+        <v>89</v>
       </c>
       <c r="H50" t="s">
-        <v>76</v>
+        <v>61</v>
       </c>
       <c r="I50" t="s">
-        <v>111</v>
+        <v>93</v>
       </c>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>97</v>
+        <v>79</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="C51" s="2"/>
       <c r="E51" t="s">
-        <v>104</v>
+        <v>86</v>
       </c>
       <c r="F51" t="s">
-        <v>107</v>
+        <v>89</v>
       </c>
       <c r="G51" t="s">
-        <v>76</v>
+        <v>61</v>
       </c>
       <c r="H51" t="s">
-        <v>76</v>
+        <v>61</v>
       </c>
       <c r="I51" t="s">
-        <v>111</v>
+        <v>93</v>
       </c>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.2">
@@ -2002,6 +2032,7 @@
       <c r="C65" s="2"/>
     </row>
   </sheetData>
+  <autoFilter ref="A1:I51" xr:uid="{5E298A3A-22C5-B847-8E38-6094955752D9}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C39">
     <sortCondition ref="A1:A39"/>
   </sortState>

</xml_diff>

<commit_message>
Add table 4/5/6/7 weekend table data
</commit_message>
<xml_diff>
--- a/InputExcel.xlsx
+++ b/InputExcel.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/justinfuentes/Desktop/Coding Projects/Hatch/b21-check/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26643C36-35D3-114D-B240-1FBA2B442266}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3573F15A-614C-9749-A7E0-054F77A23ADC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4580" yWindow="1260" windowWidth="21520" windowHeight="17560" xr2:uid="{79B376A1-3268-2549-BAEC-B5E1066DF9A0}"/>
+    <workbookView xWindow="0" yWindow="1240" windowWidth="27920" windowHeight="17560" xr2:uid="{79B376A1-3268-2549-BAEC-B5E1066DF9A0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="352" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="683" uniqueCount="129">
   <si>
     <t>Train_ID</t>
   </si>
@@ -324,9 +324,6 @@
     <t>BusinessDay</t>
   </si>
   <si>
-    <t>Ignore</t>
-  </si>
-  <si>
     <t>VIA50&amp;60</t>
   </si>
   <si>
@@ -397,16 +394,62 @@
   </si>
   <si>
     <t>21:50:00</t>
+  </si>
+  <si>
+    <t>VIA655</t>
+  </si>
+  <si>
+    <t>09:14:00</t>
+  </si>
+  <si>
+    <t>Table 3</t>
+  </si>
+  <si>
+    <t>VIA641</t>
+  </si>
+  <si>
+    <t>11:03:00</t>
+  </si>
+  <si>
+    <t>WeekendDay</t>
+  </si>
+  <si>
+    <t>Table 4</t>
+  </si>
+  <si>
+    <t>VIA643</t>
+  </si>
+  <si>
+    <t>13:18:00</t>
+  </si>
+  <si>
+    <t>10:03:00</t>
+  </si>
+  <si>
+    <t>20:18:00</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -438,11 +481,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -757,16 +803,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E298A3A-22C5-B847-8E38-6094955752D9}">
-  <dimension ref="A1:I65"/>
+  <dimension ref="A1:J115"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="27.33203125" customWidth="1"/>
-    <col min="3" max="3" width="23.5" customWidth="1"/>
+    <col min="2" max="2" width="13.83203125" customWidth="1"/>
+    <col min="3" max="3" width="16.5" customWidth="1"/>
+    <col min="4" max="4" width="12" customWidth="1"/>
+    <col min="8" max="8" width="12" customWidth="1"/>
+    <col min="9" max="9" width="13.1640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">
@@ -799,7 +848,7 @@
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+      <c r="A2" s="3" t="s">
         <v>58</v>
       </c>
       <c r="B2" s="2"/>
@@ -819,11 +868,11 @@
         <v>61</v>
       </c>
       <c r="I2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+      <c r="A3" s="3" t="s">
         <v>57</v>
       </c>
       <c r="B3" s="2" t="s">
@@ -843,7 +892,7 @@
         <v>61</v>
       </c>
       <c r="I3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
@@ -852,7 +901,7 @@
       </c>
       <c r="B4" s="2"/>
       <c r="C4" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D4" t="s">
         <v>61</v>
@@ -897,7 +946,7 @@
       </c>
       <c r="B6" s="2"/>
       <c r="C6" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D6" t="s">
         <v>61</v>
@@ -920,7 +969,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C7" s="1"/>
       <c r="D7" t="s">
@@ -948,7 +997,7 @@
       </c>
       <c r="B8" s="2"/>
       <c r="C8" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D8" t="s">
         <v>61</v>
@@ -996,7 +1045,7 @@
       </c>
       <c r="B10" s="2"/>
       <c r="C10" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D10" t="s">
         <v>61</v>
@@ -1044,7 +1093,7 @@
       </c>
       <c r="B12" s="2"/>
       <c r="C12" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D12" t="s">
         <v>61</v>
@@ -1064,7 +1113,7 @@
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B13" s="2"/>
       <c r="C13" s="2" t="s">
@@ -1115,11 +1164,11 @@
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B15" s="2"/>
       <c r="C15" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D15" t="s">
         <v>61</v>
@@ -1164,7 +1213,7 @@
       </c>
       <c r="B17" s="2"/>
       <c r="C17" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D17" t="s">
         <v>61</v>
@@ -1290,7 +1339,7 @@
       </c>
       <c r="B22" s="2"/>
       <c r="C22" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D22" t="s">
         <v>61</v>
@@ -1314,7 +1363,7 @@
       </c>
       <c r="B23" s="2"/>
       <c r="C23" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D23" t="s">
         <v>61</v>
@@ -1337,7 +1386,7 @@
         <v>15</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C24" s="1"/>
       <c r="E24" t="s">
@@ -1359,7 +1408,7 @@
       </c>
       <c r="B25" s="2"/>
       <c r="C25" s="2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E25" t="s">
         <v>85</v>
@@ -1409,7 +1458,7 @@
         <v>12</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C27" s="1"/>
       <c r="D27" t="s">
@@ -1434,7 +1483,7 @@
       </c>
       <c r="B28" s="2"/>
       <c r="C28" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E28" t="s">
         <v>85</v>
@@ -1479,7 +1528,7 @@
       </c>
       <c r="B30" s="2"/>
       <c r="C30" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D30" t="s">
         <v>61</v>
@@ -1503,7 +1552,7 @@
       </c>
       <c r="B31" s="2"/>
       <c r="C31" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D31" t="s">
         <v>61</v>
@@ -1550,7 +1599,7 @@
         <v>14</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C33" s="1"/>
       <c r="E33" t="s">
@@ -1572,7 +1621,7 @@
       </c>
       <c r="B34" s="2"/>
       <c r="C34" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D34" t="s">
         <v>61</v>
@@ -1598,7 +1647,7 @@
         <v>17</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C35" s="1"/>
       <c r="E35" t="s">
@@ -1847,7 +1896,7 @@
         <v>73</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C46" s="2"/>
       <c r="E46" t="s">
@@ -1871,7 +1920,7 @@
         <v>74</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C47" s="2"/>
       <c r="E47" t="s">
@@ -1895,7 +1944,7 @@
         <v>75</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C48" s="2"/>
       <c r="E48" t="s">
@@ -1978,79 +2027,1391 @@
       </c>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B52" s="2"/>
+      <c r="A52" t="s">
+        <v>118</v>
+      </c>
+      <c r="B52" s="2" t="s">
+        <v>119</v>
+      </c>
       <c r="C52" s="2"/>
+      <c r="E52" t="s">
+        <v>120</v>
+      </c>
+      <c r="F52" t="s">
+        <v>89</v>
+      </c>
+      <c r="G52" t="s">
+        <v>61</v>
+      </c>
+      <c r="H52" t="s">
+        <v>61</v>
+      </c>
+      <c r="I52" t="s">
+        <v>123</v>
+      </c>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B53" s="2"/>
+      <c r="A53" t="s">
+        <v>121</v>
+      </c>
+      <c r="B53" s="2" t="s">
+        <v>122</v>
+      </c>
       <c r="C53" s="2"/>
+      <c r="D53" t="s">
+        <v>61</v>
+      </c>
+      <c r="E53" t="s">
+        <v>120</v>
+      </c>
+      <c r="F53" t="s">
+        <v>89</v>
+      </c>
+      <c r="H53" t="s">
+        <v>61</v>
+      </c>
+      <c r="I53" t="s">
+        <v>123</v>
+      </c>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B54" s="2"/>
+      <c r="A54" t="s">
+        <v>7</v>
+      </c>
+      <c r="B54" s="2" t="s">
+        <v>23</v>
+      </c>
       <c r="C54" s="2"/>
+      <c r="E54" t="s">
+        <v>120</v>
+      </c>
+      <c r="F54" t="s">
+        <v>89</v>
+      </c>
+      <c r="H54" t="s">
+        <v>61</v>
+      </c>
+      <c r="I54" t="s">
+        <v>123</v>
+      </c>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B55" s="2"/>
+      <c r="A55" t="s">
+        <v>125</v>
+      </c>
+      <c r="B55" s="2" t="s">
+        <v>126</v>
+      </c>
       <c r="C55" s="2"/>
+      <c r="D55" t="s">
+        <v>61</v>
+      </c>
+      <c r="E55" t="s">
+        <v>120</v>
+      </c>
+      <c r="F55" t="s">
+        <v>89</v>
+      </c>
+      <c r="G55" t="s">
+        <v>61</v>
+      </c>
+      <c r="H55" t="s">
+        <v>61</v>
+      </c>
+      <c r="I55" t="s">
+        <v>123</v>
+      </c>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B56" s="2"/>
+      <c r="A56" t="s">
+        <v>9</v>
+      </c>
+      <c r="B56" s="2" t="s">
+        <v>25</v>
+      </c>
       <c r="C56" s="2"/>
+      <c r="E56" t="s">
+        <v>120</v>
+      </c>
+      <c r="F56" t="s">
+        <v>89</v>
+      </c>
+      <c r="H56" t="s">
+        <v>61</v>
+      </c>
+      <c r="I56" t="s">
+        <v>123</v>
+      </c>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B57" s="2"/>
+      <c r="A57" t="s">
+        <v>10</v>
+      </c>
+      <c r="B57" s="2" t="s">
+        <v>26</v>
+      </c>
       <c r="C57" s="2"/>
+      <c r="E57" t="s">
+        <v>120</v>
+      </c>
+      <c r="F57" t="s">
+        <v>89</v>
+      </c>
+      <c r="G57" t="s">
+        <v>61</v>
+      </c>
+      <c r="H57" t="s">
+        <v>61</v>
+      </c>
+      <c r="I57" t="s">
+        <v>123</v>
+      </c>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B58" s="2"/>
+      <c r="A58" t="s">
+        <v>4</v>
+      </c>
+      <c r="B58" s="2" t="s">
+        <v>127</v>
+      </c>
       <c r="C58" s="2"/>
+      <c r="E58" t="s">
+        <v>120</v>
+      </c>
+      <c r="F58" t="s">
+        <v>89</v>
+      </c>
+      <c r="G58" t="s">
+        <v>61</v>
+      </c>
+      <c r="H58" t="s">
+        <v>61</v>
+      </c>
+      <c r="I58" t="s">
+        <v>123</v>
+      </c>
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B59" s="2"/>
+      <c r="A59" t="s">
+        <v>11</v>
+      </c>
+      <c r="B59" s="2" t="s">
+        <v>27</v>
+      </c>
       <c r="C59" s="2"/>
+      <c r="E59" t="s">
+        <v>120</v>
+      </c>
+      <c r="F59" t="s">
+        <v>89</v>
+      </c>
+      <c r="H59" t="s">
+        <v>61</v>
+      </c>
+      <c r="I59" t="s">
+        <v>123</v>
+      </c>
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B60" s="2"/>
+      <c r="A60" t="s">
+        <v>12</v>
+      </c>
+      <c r="B60" s="2" t="s">
+        <v>97</v>
+      </c>
       <c r="C60" s="2"/>
+      <c r="D60" t="s">
+        <v>61</v>
+      </c>
+      <c r="E60" t="s">
+        <v>120</v>
+      </c>
+      <c r="F60" t="s">
+        <v>89</v>
+      </c>
+      <c r="H60" t="s">
+        <v>61</v>
+      </c>
+      <c r="I60" t="s">
+        <v>123</v>
+      </c>
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B61" s="2"/>
+      <c r="A61" t="s">
+        <v>13</v>
+      </c>
+      <c r="B61" s="2" t="s">
+        <v>28</v>
+      </c>
       <c r="C61" s="2"/>
+      <c r="E61" t="s">
+        <v>120</v>
+      </c>
+      <c r="F61" t="s">
+        <v>89</v>
+      </c>
+      <c r="G61" t="s">
+        <v>61</v>
+      </c>
+      <c r="H61" t="s">
+        <v>61</v>
+      </c>
+      <c r="I61" t="s">
+        <v>123</v>
+      </c>
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B62" s="2"/>
+      <c r="A62" t="s">
+        <v>14</v>
+      </c>
+      <c r="B62" s="2" t="s">
+        <v>98</v>
+      </c>
       <c r="C62" s="2"/>
+      <c r="E62" t="s">
+        <v>120</v>
+      </c>
+      <c r="F62" t="s">
+        <v>89</v>
+      </c>
+      <c r="H62" t="s">
+        <v>61</v>
+      </c>
+      <c r="I62" t="s">
+        <v>123</v>
+      </c>
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B63" s="2"/>
+      <c r="A63" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B63" s="2" t="s">
+        <v>99</v>
+      </c>
       <c r="C63" s="2"/>
+      <c r="D63" s="2"/>
+      <c r="E63" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="F63" t="s">
+        <v>89</v>
+      </c>
+      <c r="G63" s="2"/>
+      <c r="H63" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="I63" t="s">
+        <v>123</v>
+      </c>
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A64" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B64" s="2" t="s">
+        <v>49</v>
+      </c>
       <c r="C64" s="2"/>
-    </row>
-    <row r="65" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="D64" s="2"/>
+      <c r="E64" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="F64" t="s">
+        <v>89</v>
+      </c>
+      <c r="G64" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="H64" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="I64" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="65" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A65" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B65" s="2" t="s">
+        <v>100</v>
+      </c>
       <c r="C65" s="2"/>
+      <c r="D65" s="2"/>
+      <c r="E65" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="F65" t="s">
+        <v>89</v>
+      </c>
+      <c r="G65" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="H65" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="I65" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="66" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A66" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B66" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C66" s="2"/>
+      <c r="D66" s="2"/>
+      <c r="E66" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="F66" t="s">
+        <v>89</v>
+      </c>
+      <c r="G66" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="H66" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="I66" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="67" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A67" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B67" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C67" s="2"/>
+      <c r="D67" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="E67" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="F67" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="G67" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="H67" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="I67" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="68" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A68" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B68" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C68" s="2"/>
+      <c r="D68" s="2"/>
+      <c r="E68" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="F68" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="G68" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="H68" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="I68" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="69" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A69" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="C69" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="D69" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="E69" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="F69" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="G69" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="H69" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="I69" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="70" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A70" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="B70" s="2"/>
+      <c r="C70" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="D70" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="E70" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="F70" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="G70" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="H70" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="I70" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="71" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A71" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B71" s="2"/>
+      <c r="C71" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="D71" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="E71" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="F71" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="G71" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="H71" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="I71" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="72" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A72" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B72" s="2"/>
+      <c r="C72" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="D72" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="E72" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="F72" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="G72" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="H72" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="I72" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="73" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A73" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B73" s="2"/>
+      <c r="C73" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="D73" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="E73" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="F73" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="G73" s="2"/>
+      <c r="H73" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="I73" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="74" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A74" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B74" s="2"/>
+      <c r="C74" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="D74" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="E74" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="F74" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="G74" s="2"/>
+      <c r="H74" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="I74" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="75" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A75" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B75" s="2"/>
+      <c r="C75" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="D75" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="E75" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="F75" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="G75" s="2"/>
+      <c r="H75" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="I75" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="76" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A76" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B76" s="2"/>
+      <c r="C76" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="D76" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="E76" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="F76" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="G76" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="H76" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="I76" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="77" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A77" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B77" s="2"/>
+      <c r="C77" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="D77" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="E77" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="F77" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="G77" s="2"/>
+      <c r="H77" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="I77" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="78" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A78" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B78" s="2"/>
+      <c r="C78" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="D78" s="2"/>
+      <c r="E78" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="F78" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="G78" s="2"/>
+      <c r="H78" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="I78" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="79" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A79" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B79" s="2"/>
+      <c r="C79" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="D79" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="E79" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="F79" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="G79" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="H79" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="I79" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="80" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A80" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B80" s="2"/>
+      <c r="C80" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="D80" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="E80" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="F80" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="G80" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="H80" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="I80" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="81" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A81" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B81" s="2"/>
+      <c r="C81" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="D81" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="E81" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="F81" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="G81" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="H81" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="I81" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="82" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A82" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B82" s="2"/>
+      <c r="C82" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="D82" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="E82" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="F82" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="G82" s="2"/>
+      <c r="H82" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="I82" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="83" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A83" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B83" s="2"/>
+      <c r="C83" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="D83" s="2"/>
+      <c r="E83" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="F83" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="G83" s="2"/>
+      <c r="H83" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="I83" s="2" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="84" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A84" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="B84" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="D84" s="2"/>
+      <c r="E84" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="F84" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="G84" s="2"/>
+      <c r="H84" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="I84" s="2" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="85" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A85" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B85" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="D85" s="2"/>
+      <c r="E85" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="F85" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="G85" s="2"/>
+      <c r="H85" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="I85" s="2" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="86" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A86" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="B86" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="C86" s="2"/>
+      <c r="D86" s="2"/>
+      <c r="E86" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="F86" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="G86" s="2"/>
+      <c r="H86" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="I86" s="2" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="87" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A87" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="B87" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="C87" s="2"/>
+      <c r="D87" s="2"/>
+      <c r="E87" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="F87" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="G87" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="H87" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="I87" s="2" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="88" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A88" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="B88" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="C88" s="2"/>
+      <c r="D88" s="2"/>
+      <c r="E88" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="F88" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="G88" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="H88" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="I88" s="2" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="89" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A89" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="B89" s="2"/>
+      <c r="C89" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="D89" s="2"/>
+      <c r="E89" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="F89" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="G89" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="H89" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="I89" s="2" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="90" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A90" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="C90" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="D90" s="2"/>
+      <c r="E90" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="F90" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="G90" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="H90" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="I90" s="2" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="91" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A91" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="B91" s="2"/>
+      <c r="C91" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="D91" s="2"/>
+      <c r="E91" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="F91" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="G91" s="2"/>
+      <c r="H91" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="I91" s="2" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="92" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A92" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="B92" s="2"/>
+      <c r="C92" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="D92" s="2"/>
+      <c r="E92" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="F92" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="G92" s="2"/>
+      <c r="H92" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="I92" s="2" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="93" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A93" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B93" s="2"/>
+      <c r="C93" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="D93" s="2"/>
+      <c r="E93" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="F93" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="G93" s="2"/>
+      <c r="H93" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="I93" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="J93" s="2"/>
+    </row>
+    <row r="94" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A94" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="B94" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C94" s="2"/>
+      <c r="E94" t="s">
+        <v>84</v>
+      </c>
+      <c r="F94" t="s">
+        <v>89</v>
+      </c>
+      <c r="H94" t="s">
+        <v>61</v>
+      </c>
+      <c r="I94" t="s">
+        <v>123</v>
+      </c>
+      <c r="J94" s="2"/>
+    </row>
+    <row r="95" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A95" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="B95" s="2"/>
+      <c r="C95" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="E95" t="s">
+        <v>84</v>
+      </c>
+      <c r="F95" t="s">
+        <v>88</v>
+      </c>
+      <c r="G95" t="s">
+        <v>61</v>
+      </c>
+      <c r="H95" t="s">
+        <v>61</v>
+      </c>
+      <c r="I95" t="s">
+        <v>123</v>
+      </c>
+      <c r="J95" s="2"/>
+    </row>
+    <row r="96" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A96" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="B96" s="2"/>
+      <c r="C96" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="E96" t="s">
+        <v>84</v>
+      </c>
+      <c r="F96" t="s">
+        <v>88</v>
+      </c>
+      <c r="H96" t="s">
+        <v>61</v>
+      </c>
+      <c r="I96" t="s">
+        <v>123</v>
+      </c>
+      <c r="J96" s="2"/>
+    </row>
+    <row r="97" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A97" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="B97" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="C97" s="2"/>
+      <c r="E97" t="s">
+        <v>84</v>
+      </c>
+      <c r="F97" t="s">
+        <v>89</v>
+      </c>
+      <c r="G97" t="s">
+        <v>61</v>
+      </c>
+      <c r="H97" t="s">
+        <v>61</v>
+      </c>
+      <c r="I97" t="s">
+        <v>123</v>
+      </c>
+      <c r="J97" s="2"/>
+    </row>
+    <row r="98" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A98" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="B98" s="5"/>
+      <c r="C98" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="D98" s="4"/>
+      <c r="E98" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="F98" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="G98" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="H98" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="I98" t="s">
+        <v>123</v>
+      </c>
+      <c r="J98" s="2"/>
+    </row>
+    <row r="99" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A99" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="B99" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="C99" s="5"/>
+      <c r="D99" s="4"/>
+      <c r="E99" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="F99" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="G99" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="H99" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="I99" t="s">
+        <v>123</v>
+      </c>
+      <c r="J99" s="2"/>
+    </row>
+    <row r="100" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A100" s="2"/>
+      <c r="B100" s="2"/>
+      <c r="C100" s="2"/>
+      <c r="D100" s="2"/>
+      <c r="E100" s="2"/>
+      <c r="F100" s="2"/>
+      <c r="G100" s="2"/>
+      <c r="H100" s="2"/>
+      <c r="I100" s="2"/>
+      <c r="J100" s="2"/>
+    </row>
+    <row r="101" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A101" s="2"/>
+      <c r="B101" s="2"/>
+      <c r="C101" s="2"/>
+      <c r="D101" s="2"/>
+      <c r="E101" s="2"/>
+      <c r="F101" s="2"/>
+      <c r="G101" s="2"/>
+      <c r="H101" s="2"/>
+      <c r="I101" s="2"/>
+      <c r="J101" s="2"/>
+    </row>
+    <row r="102" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A102" s="2"/>
+      <c r="B102" s="2"/>
+      <c r="C102" s="2"/>
+      <c r="D102" s="2"/>
+      <c r="E102" s="2"/>
+      <c r="F102" s="2"/>
+      <c r="G102" s="2"/>
+      <c r="H102" s="2"/>
+      <c r="I102" s="2"/>
+      <c r="J102" s="2"/>
+    </row>
+    <row r="103" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A103" s="2"/>
+      <c r="B103" s="2"/>
+      <c r="C103" s="2"/>
+      <c r="D103" s="2"/>
+      <c r="E103" s="2"/>
+      <c r="F103" s="2"/>
+      <c r="G103" s="2"/>
+      <c r="H103" s="2"/>
+      <c r="I103" s="2"/>
+      <c r="J103" s="2"/>
+    </row>
+    <row r="104" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A104" s="2"/>
+      <c r="B104" s="2"/>
+      <c r="C104" s="2"/>
+      <c r="D104" s="2"/>
+      <c r="E104" s="2"/>
+      <c r="F104" s="2"/>
+      <c r="G104" s="2"/>
+      <c r="H104" s="2"/>
+      <c r="I104" s="2"/>
+      <c r="J104" s="2"/>
+    </row>
+    <row r="105" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A105" s="2"/>
+      <c r="B105" s="2"/>
+      <c r="C105" s="2"/>
+      <c r="D105" s="2"/>
+      <c r="E105" s="2"/>
+      <c r="F105" s="2"/>
+      <c r="G105" s="2"/>
+      <c r="H105" s="2"/>
+      <c r="I105" s="2"/>
+      <c r="J105" s="2"/>
+    </row>
+    <row r="106" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A106" s="2"/>
+      <c r="B106" s="2"/>
+      <c r="C106" s="2"/>
+      <c r="D106" s="2"/>
+      <c r="E106" s="2"/>
+      <c r="F106" s="2"/>
+      <c r="G106" s="2"/>
+      <c r="H106" s="2"/>
+      <c r="I106" s="2"/>
+      <c r="J106" s="2"/>
+    </row>
+    <row r="107" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A107" s="2"/>
+      <c r="B107" s="2"/>
+      <c r="C107" s="2"/>
+      <c r="D107" s="2"/>
+      <c r="E107" s="2"/>
+      <c r="F107" s="2"/>
+      <c r="G107" s="2"/>
+      <c r="H107" s="2"/>
+      <c r="I107" s="2"/>
+      <c r="J107" s="2"/>
+    </row>
+    <row r="108" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A108" s="2"/>
+      <c r="B108" s="2"/>
+      <c r="C108" s="2"/>
+      <c r="D108" s="2"/>
+      <c r="E108" s="2"/>
+      <c r="F108" s="2"/>
+      <c r="G108" s="2"/>
+      <c r="H108" s="2"/>
+      <c r="I108" s="2"/>
+      <c r="J108" s="2"/>
+    </row>
+    <row r="109" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A109" s="2"/>
+      <c r="B109" s="2"/>
+      <c r="C109" s="2"/>
+      <c r="D109" s="2"/>
+      <c r="E109" s="2"/>
+      <c r="F109" s="2"/>
+      <c r="G109" s="2"/>
+      <c r="H109" s="2"/>
+      <c r="I109" s="2"/>
+      <c r="J109" s="2"/>
+    </row>
+    <row r="110" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A110" s="2"/>
+      <c r="B110" s="2"/>
+      <c r="C110" s="2"/>
+      <c r="D110" s="2"/>
+      <c r="E110" s="2"/>
+      <c r="F110" s="2"/>
+      <c r="G110" s="2"/>
+      <c r="H110" s="2"/>
+      <c r="I110" s="2"/>
+      <c r="J110" s="2"/>
+    </row>
+    <row r="111" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A111" s="2"/>
+      <c r="B111" s="2"/>
+      <c r="C111" s="2"/>
+      <c r="D111" s="2"/>
+      <c r="E111" s="2"/>
+      <c r="F111" s="2"/>
+      <c r="G111" s="2"/>
+      <c r="H111" s="2"/>
+      <c r="I111" s="2"/>
+      <c r="J111" s="2"/>
+    </row>
+    <row r="112" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A112" s="2"/>
+      <c r="B112" s="2"/>
+      <c r="C112" s="2"/>
+      <c r="D112" s="2"/>
+      <c r="E112" s="2"/>
+      <c r="F112" s="2"/>
+      <c r="G112" s="2"/>
+      <c r="H112" s="2"/>
+      <c r="I112" s="2"/>
+      <c r="J112" s="2"/>
+    </row>
+    <row r="113" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A113" s="2"/>
+      <c r="B113" s="2"/>
+      <c r="C113" s="2"/>
+      <c r="D113" s="2"/>
+      <c r="E113" s="2"/>
+      <c r="F113" s="2"/>
+      <c r="G113" s="2"/>
+      <c r="H113" s="2"/>
+      <c r="I113" s="2"/>
+      <c r="J113" s="2"/>
+    </row>
+    <row r="114" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A114" s="2"/>
+      <c r="B114" s="2"/>
+      <c r="C114" s="2"/>
+      <c r="D114" s="2"/>
+      <c r="E114" s="2"/>
+      <c r="F114" s="2"/>
+      <c r="G114" s="2"/>
+      <c r="H114" s="2"/>
+      <c r="I114" s="2"/>
+      <c r="J114" s="2"/>
+    </row>
+    <row r="115" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A115" s="2"/>
+      <c r="B115" s="2"/>
+      <c r="C115" s="2"/>
+      <c r="D115" s="2"/>
+      <c r="E115" s="2"/>
+      <c r="F115" s="2"/>
+      <c r="G115" s="2"/>
+      <c r="H115" s="2"/>
+      <c r="I115" s="2"/>
+      <c r="J115" s="2"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:I51" xr:uid="{5E298A3A-22C5-B847-8E38-6094955752D9}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C39">
     <sortCondition ref="A1:A39"/>
   </sortState>
+  <phoneticPr fontId="1" type="noConversion"/>
   <dataValidations count="5">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E1" xr:uid="{21FFFA42-49BF-654D-973B-24FD3A7A6AC9}">
       <formula1>"Table 1,Table 2,Table 3,Table 4,Table 5, Table 6,Table 7"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E1048576" xr:uid="{ABABF387-24A1-614F-94D2-C99F2EFF2DFA}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E97 E100:E1048576" xr:uid="{ABABF387-24A1-614F-94D2-C99F2EFF2DFA}">
       <formula1>"Table 1,Table 2,Table 3,Table 4,Table 5,Table 6,Table 7"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F1:F1048576" xr:uid="{3F3C557A-EEA1-4F4F-BF22-0F7CFA220DC2}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F1:F97 F100:F1048576" xr:uid="{3F3C557A-EEA1-4F4F-BF22-0F7CFA220DC2}">
       <formula1>"Outbound,Inbound"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G1048576" xr:uid="{D8696CB5-2EF9-EE46-9890-299C7E2A49B1}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G97 G100:G1048576" xr:uid="{D8696CB5-2EF9-EE46-9890-299C7E2A49B1}">
       <formula1>"yes"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I2:I102" xr:uid="{91EAA47F-B2BD-0E4B-803E-80401D46D9FC}">
-      <formula1>"Special,Both,BusinessDay,Ignore"</formula1>
+      <formula1>"Special,Both,BusinessDay,Ignore,WeekendDay"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Add minor AUG 1 changes
</commit_message>
<xml_diff>
--- a/InputExcel.xlsx
+++ b/InputExcel.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/justinfuentes/Desktop/Coding Projects/Hatch/b21-check/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3573F15A-614C-9749-A7E0-054F77A23ADC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B6DBED9-7329-D24F-AB4A-01DC62F0CED5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1240" windowWidth="27920" windowHeight="17560" xr2:uid="{79B376A1-3268-2549-BAEC-B5E1066DF9A0}"/>
+    <workbookView xWindow="320" yWindow="760" windowWidth="27920" windowHeight="17560" xr2:uid="{79B376A1-3268-2549-BAEC-B5E1066DF9A0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="683" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="689" uniqueCount="130">
   <si>
     <t>Train_ID</t>
   </si>
@@ -427,6 +427,9 @@
   </si>
   <si>
     <t>20:18:00</t>
+  </si>
+  <si>
+    <t>VIA81</t>
   </si>
 </sst>
 </file>
@@ -803,19 +806,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E298A3A-22C5-B847-8E38-6094955752D9}">
-  <dimension ref="A1:J115"/>
+  <dimension ref="A1:J116"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="13.83203125" customWidth="1"/>
+    <col min="2" max="2" width="13.33203125" customWidth="1"/>
     <col min="3" max="3" width="16.5" customWidth="1"/>
-    <col min="4" max="4" width="12" customWidth="1"/>
-    <col min="8" max="8" width="12" customWidth="1"/>
-    <col min="9" max="9" width="13.1640625" customWidth="1"/>
+    <col min="4" max="4" width="11.83203125" customWidth="1"/>
+    <col min="5" max="5" width="8.5" customWidth="1"/>
+    <col min="6" max="6" width="9.83203125" customWidth="1"/>
+    <col min="8" max="8" width="11.5" customWidth="1"/>
+    <col min="9" max="9" width="12.83203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">
@@ -3031,18 +3036,18 @@
     </row>
     <row r="93" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A93" s="2" t="s">
-        <v>50</v>
+        <v>62</v>
       </c>
       <c r="B93" s="2"/>
       <c r="C93" s="2" t="s">
-        <v>51</v>
+        <v>63</v>
       </c>
       <c r="D93" s="2"/>
       <c r="E93" s="2" t="s">
-        <v>84</v>
+        <v>124</v>
       </c>
       <c r="F93" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="G93" s="2"/>
       <c r="H93" s="2" t="s">
@@ -3054,43 +3059,42 @@
       <c r="J93" s="2"/>
     </row>
     <row r="94" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A94" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="B94" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="C94" s="2"/>
-      <c r="E94" t="s">
-        <v>84</v>
-      </c>
-      <c r="F94" t="s">
-        <v>89</v>
-      </c>
-      <c r="H94" t="s">
-        <v>61</v>
-      </c>
-      <c r="I94" t="s">
+      <c r="A94" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="B94" s="2"/>
+      <c r="C94" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="D94" s="2"/>
+      <c r="E94" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="F94" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="G94" s="2"/>
+      <c r="H94" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="I94" s="2" t="s">
         <v>123</v>
       </c>
       <c r="J94" s="2"/>
     </row>
     <row r="95" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A95" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="B95" s="2"/>
-      <c r="C95" s="2" t="s">
-        <v>55</v>
-      </c>
+        <v>50</v>
+      </c>
+      <c r="B95" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C95" s="2"/>
       <c r="E95" t="s">
         <v>84</v>
       </c>
       <c r="F95" t="s">
-        <v>88</v>
-      </c>
-      <c r="G95" t="s">
-        <v>61</v>
+        <v>89</v>
       </c>
       <c r="H95" t="s">
         <v>61</v>
@@ -3102,11 +3106,11 @@
     </row>
     <row r="96" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A96" s="3" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="B96" s="2"/>
       <c r="C96" s="2" t="s">
-        <v>48</v>
+        <v>55</v>
       </c>
       <c r="E96" t="s">
         <v>84</v>
@@ -3114,6 +3118,9 @@
       <c r="F96" t="s">
         <v>88</v>
       </c>
+      <c r="G96" t="s">
+        <v>61</v>
+      </c>
       <c r="H96" t="s">
         <v>61</v>
       </c>
@@ -3124,20 +3131,17 @@
     </row>
     <row r="97" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A97" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="B97" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="C97" s="2"/>
+        <v>56</v>
+      </c>
+      <c r="B97" s="2"/>
+      <c r="C97" s="2" t="s">
+        <v>48</v>
+      </c>
       <c r="E97" t="s">
         <v>84</v>
       </c>
       <c r="F97" t="s">
-        <v>89</v>
-      </c>
-      <c r="G97" t="s">
-        <v>61</v>
+        <v>88</v>
       </c>
       <c r="H97" t="s">
         <v>61</v>
@@ -3148,24 +3152,23 @@
       <c r="J97" s="2"/>
     </row>
     <row r="98" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A98" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="B98" s="5"/>
-      <c r="C98" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="D98" s="4"/>
-      <c r="E98" s="4" t="s">
-        <v>81</v>
-      </c>
-      <c r="F98" s="4" t="s">
-        <v>88</v>
-      </c>
-      <c r="G98" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="H98" s="4" t="s">
+      <c r="A98" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="B98" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="C98" s="2"/>
+      <c r="E98" t="s">
+        <v>84</v>
+      </c>
+      <c r="F98" t="s">
+        <v>89</v>
+      </c>
+      <c r="G98" t="s">
+        <v>61</v>
+      </c>
+      <c r="H98" t="s">
         <v>61</v>
       </c>
       <c r="I98" t="s">
@@ -3175,40 +3178,54 @@
     </row>
     <row r="99" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A99" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="B99" s="5" t="s">
-        <v>82</v>
-      </c>
-      <c r="C99" s="5"/>
+        <v>58</v>
+      </c>
+      <c r="B99" s="5"/>
+      <c r="C99" s="5" t="s">
+        <v>59</v>
+      </c>
       <c r="D99" s="4"/>
       <c r="E99" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="F99" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="G99" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="H99" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="I99" t="s">
+        <v>123</v>
+      </c>
+      <c r="J99" s="2"/>
+    </row>
+    <row r="100" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A100" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="B100" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="C100" s="5"/>
+      <c r="D100" s="4"/>
+      <c r="E100" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="F99" s="4" t="s">
-        <v>89</v>
-      </c>
-      <c r="G99" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="H99" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="I99" t="s">
-        <v>123</v>
-      </c>
-      <c r="J99" s="2"/>
-    </row>
-    <row r="100" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A100" s="2"/>
-      <c r="B100" s="2"/>
-      <c r="C100" s="2"/>
-      <c r="D100" s="2"/>
-      <c r="E100" s="2"/>
-      <c r="F100" s="2"/>
-      <c r="G100" s="2"/>
-      <c r="H100" s="2"/>
-      <c r="I100" s="2"/>
+      <c r="F100" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="G100" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="H100" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="I100" t="s">
+        <v>123</v>
+      </c>
       <c r="J100" s="2"/>
     </row>
     <row r="101" spans="1:10" x14ac:dyDescent="0.2">
@@ -3391,6 +3408,18 @@
       <c r="I115" s="2"/>
       <c r="J115" s="2"/>
     </row>
+    <row r="116" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A116" s="2"/>
+      <c r="B116" s="2"/>
+      <c r="C116" s="2"/>
+      <c r="D116" s="2"/>
+      <c r="E116" s="2"/>
+      <c r="F116" s="2"/>
+      <c r="G116" s="2"/>
+      <c r="H116" s="2"/>
+      <c r="I116" s="2"/>
+      <c r="J116" s="2"/>
+    </row>
   </sheetData>
   <autoFilter ref="A1:I51" xr:uid="{5E298A3A-22C5-B847-8E38-6094955752D9}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C39">
@@ -3401,16 +3430,16 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E1" xr:uid="{21FFFA42-49BF-654D-973B-24FD3A7A6AC9}">
       <formula1>"Table 1,Table 2,Table 3,Table 4,Table 5, Table 6,Table 7"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E97 E100:E1048576" xr:uid="{ABABF387-24A1-614F-94D2-C99F2EFF2DFA}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E101:E1048576 E2:E98" xr:uid="{ABABF387-24A1-614F-94D2-C99F2EFF2DFA}">
       <formula1>"Table 1,Table 2,Table 3,Table 4,Table 5,Table 6,Table 7"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F1:F97 F100:F1048576" xr:uid="{3F3C557A-EEA1-4F4F-BF22-0F7CFA220DC2}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F101:F1048576 F1:F98" xr:uid="{3F3C557A-EEA1-4F4F-BF22-0F7CFA220DC2}">
       <formula1>"Outbound,Inbound"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G97 G100:G1048576" xr:uid="{D8696CB5-2EF9-EE46-9890-299C7E2A49B1}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G101:G1048576 G2:G98" xr:uid="{D8696CB5-2EF9-EE46-9890-299C7E2A49B1}">
       <formula1>"yes"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I2:I102" xr:uid="{91EAA47F-B2BD-0E4B-803E-80401D46D9FC}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I2:I103" xr:uid="{91EAA47F-B2BD-0E4B-803E-80401D46D9FC}">
       <formula1>"Special,Both,BusinessDay,Ignore,WeekendDay"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>